<commit_message>
S03/G01: Strategy service: metadata and parameter storage
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<ns0:sst xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="154">
+<ns0:sst xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="157">
   <ns0:si>
     <ns0:t xml:space="preserve">sprint#</ns0:t>
   </ns0:si>
@@ -482,6 +482,491 @@
   </ns0:si>
   <ns0:si>
     <ns0:t xml:space="preserve">Price and volume preview charts (recharts) backed by preview API added.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Strategy CRUD API endpoints implemented.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Strategy parameter CRUD endpoints wired to strategies.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Tags/category/status/integration fields exposed in API models.</ns0:t>
+  </ns0:si>
+</ns0:sst>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<ns0:sst xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="157">
+  <ns0:si>
+    <ns0:t xml:space="preserve">sprint#</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">group#</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">group task description</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">task#</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">task description</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">remarks</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">status</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">deviations (from original plan)</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">G01</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Backend foundation: FastAPI skeleton, config, meta DB setup</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G01_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Create FastAPI project skeleton with basic app factory and routing structure.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">implemented</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G01_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement configuration loader (env-based) for DB paths, Kite keys, and app settings.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G01_TB003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Design and create sigmaqlab_meta.db schema migration for core tables (strategies, strategy_parameters, backtests).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G01_TB004</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Set up structured logging for backend (JSON or key-value format) with log levels and request logging.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">G02</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Frontend foundation: React+TS+MUI scaffold and base layout</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G02_TF001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Create React + TypeScript + Vite (or CRA) app and integrate Material UI.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G02_TF002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement global layout: AppBar with SigmaQLab branding, navigation skeleton, and basic dark theme.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G02_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Set up React Router with routes for Dashboard, Strategies, Backtests, Data, Settings.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">G03</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Developer experience: tooling, linting, and pre-commit</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G03_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Configure backend tooling: black, isort, mypy/ruff, and add pre-commit hooks.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G03_TF002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Configure frontend tooling: ESLint, Prettier, TypeScript strict settings.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S01_G03_TB003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add basic test harness for backend (pytest) with one sample test to validate CI wiring.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Data service: Kite/yfinance integration and price DB persistence</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G01_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Zerodha Kite client wrapper for historical OHLCV and holdings (read-only).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G01_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement optional yfinance/CSV loader as fallback data provider.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G01_TB003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Design and create sigmaqlab_prices.db schema (price_bars table with indices).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G01_TB004</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Data Service functions to fetch, normalize, and persist OHLCV data from providers into price DB.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G01_TB005</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Expose FastAPI endpoint to trigger data fetch for given symbol, timeframe, and date range.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Data management UI: fetch, list, and preview data</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G02_TF001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Create Data page with form to trigger data fetch via API (symbol, timeframe, date range).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">pending</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G02_TF002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement table listing available symbol/timeframe combinations and coverage ranges.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S02_G02_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add simple price &amp; volume preview chart for selected symbol/timeframe using chosen charting library.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S03</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Strategy service: metadata and parameter storage</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S03_G01_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Strategy CRUD endpoints (create, list, get, update, delete) in FastAPI.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S03_G01_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Strategy Parameters CRUD endpoints and tie them to strategies.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S03_G01_TB003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add fields for tags, categories, statuses, and integration metadata in schema and API models.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Strategy Library UI: list, details, and parameter sets</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S03_G02_TF001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Strategies list view with filters (status, category, search) and pagination.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S03_G02_TF002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Strategy detail view showing description, tags, and recent backtests placeholder.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S03_G02_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add parameter set management UI (list, create, edit, delete) for each strategy.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S04</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Backtest engine: Backtrader integration and engine interface</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S04_G01_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Define Strategy Engine interface and BacktestResult data models in backend.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S04_G01_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Integrate Backtrader as primary engine and implement adapter that conforms to engine interface.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S04_G01_TB003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement one reference strategy in Backtrader (e.g., simple SMA crossover) wired to a Strategy record.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Backtest execution: API endpoint and simple UI trigger</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S04_G02_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement API to run a single backtest given strategy_id, params_id, symbols, timeframe, and date range.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S04_G02_TF002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add 'Run Backtest' modal/dialog in Strategy detail view to configure and submit a backtest.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S04_G02_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Create basic Backtests list page showing submitted runs, status, and key summary fields.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S05</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Backtest results: persistence and metrics calculation</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S05_G01_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Persist equity curve and trades from Backtrader runs into backtest_equity_points and backtest_trades tables.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S05_G01_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Compute key metrics (total return, max drawdown, win rate, average win/loss, trade count) and store in metrics_json.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S05_G01_TB003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Expose API endpoints to fetch backtest summary, equity series, and trades for a given backtest_id.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Backtest detail UI: equity chart, trades table, and parameters</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S05_G02_TF001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Backtest detail page with summary metrics and equity curve chart (interactive).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S05_G02_TF002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add trades table with sorting/filtering, showing entry/exit, P&amp;L, and basic stats.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S05_G02_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Optionally overlay buy/sell markers on price chart for one-symbol backtests.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S06</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Batch backtesting: grid search and parallel execution</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S06_G01_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Extend backtest API to accept parameter grids or multiple parameter sets for batch execution.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S06_G01_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement batch execution using ProcessPoolExecutor with isolation per run.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S06_G01_TB003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Store batch group identifier to link multiple backtests that belong to one optimization run.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Optimization UI: batch backtests and parameter-performance views</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S06_G02_TF001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Create UI to configure and submit batch backtests (parameter ranges, symbol universe).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S06_G02_TF002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement batch results view showing parameter combinations and key metrics in tabular form.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S06_G02_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add simple visualization (e.g., heatmap or scatter plot) of parameters vs performance.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Portfolio snapshots: schema, API, and import from Kite</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G01_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Create portfolio_snapshots schema and CRUD endpoints for storing holdings snapshots.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G01_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement Data Service function to import current holdings from Kite into a portfolio snapshot.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G01_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Add Portfolio page UI to list snapshots and show holdings with core/tactical tagging controls.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Portfolio-aware backtests: starting portfolio and constraints</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G02_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Extend backtest engine config to accept a starting portfolio snapshot and core/tactical constraints.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G02_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Update metrics to report portfolio-level impact (realized + unrealized changes vs baseline).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G02_TF003</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Update Backtest configuration UI to allow selecting a portfolio snapshot when running a backtest.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Integration hooks: expose strategy summaries for SigmaTrader</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G03_TB001</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Implement read-only API endpoint to return latest backtest summary for a given strategy_id for external consumers (SigmaTrader).</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">S07_G03_TB002</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Ensure strategies can store and display linked SigmaTrader IDs and TradingView templates in the UI.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">FastAPI app factory and /health endpoint created.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Env-based Settings config using pydantic-settings added.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">sigmaqlab_meta.db schema for strategies/params/backtests wired via SQLAlchemy.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">JSON logging with level/timestamp and Uvicorn integration configured.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">React + TS + Vite + MUI frontend scaffolded.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Global dark theme and SigmaQLab layout (AppBar + nav) implemented.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">React Router routes for Dashboard/Strategies/Backtests/Data/Settings added.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Backend tooling (black, ruff, pytest, pre-commit) configured.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Frontend tooling (ESLint, Prettier, strict TS) configured.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Basic pytest harness with /health test in place.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Kite client wrapper for historical OHLCV implemented.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">yfinance and CSV data providers added as fallbacks.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">sigmaqlab_prices.db and price_bars schema created.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">DataService to fetch/normalise/persist OHLCV into prices DB implemented.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">/api/data/fetch endpoint added and covered by tests.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Data page fetch form wired to backend data fetch API.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Coverage summary table listing symbol/exchange/timeframe and coverage added.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Price and volume preview charts (recharts) backed by preview API added.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Strategy CRUD API endpoints implemented.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Strategy parameter CRUD endpoints wired to strategies.</ns0:t>
+  </ns0:si>
+  <ns0:si>
+    <ns0:t xml:space="preserve">Tags/category/status/integration fields exposed in API models.</ns0:t>
   </ns0:si>
 </ns0:sst>
 </file>
@@ -1318,7 +1803,10 @@
         <ns0:v>59</ns0:v>
       </ns0:c>
       <ns0:c r="G20" s="1" t="s">
-        <ns0:v>51</ns0:v>
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F20" s="1" t="s">
+        <ns0:v>154</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1338,7 +1826,10 @@
         <ns0:v>61</ns0:v>
       </ns0:c>
       <ns0:c r="G21" s="1" t="s">
-        <ns0:v>51</ns0:v>
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F21" s="1" t="s">
+        <ns0:v>155</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,7 +1849,1133 @@
         <ns0:v>63</ns0:v>
       </ns0:c>
       <ns0:c r="G22" s="1" t="s">
-        <ns0:v>51</ns0:v>
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F22" s="1" t="s">
+        <ns0:v>156</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A23" s="1" t="s">
+        <ns0:v>56</ns0:v>
+      </ns0:c>
+      <ns0:c r="B23" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C23" s="1" t="s">
+        <ns0:v>64</ns0:v>
+      </ns0:c>
+      <ns0:c r="D23" s="1" t="s">
+        <ns0:v>65</ns0:v>
+      </ns0:c>
+      <ns0:c r="E23" s="1" t="s">
+        <ns0:v>66</ns0:v>
+      </ns0:c>
+      <ns0:c r="G23" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A24" s="1" t="s">
+        <ns0:v>56</ns0:v>
+      </ns0:c>
+      <ns0:c r="B24" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C24" s="1" t="s">
+        <ns0:v>64</ns0:v>
+      </ns0:c>
+      <ns0:c r="D24" s="1" t="s">
+        <ns0:v>67</ns0:v>
+      </ns0:c>
+      <ns0:c r="E24" s="1" t="s">
+        <ns0:v>68</ns0:v>
+      </ns0:c>
+      <ns0:c r="G24" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A25" s="1" t="s">
+        <ns0:v>56</ns0:v>
+      </ns0:c>
+      <ns0:c r="B25" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C25" s="1" t="s">
+        <ns0:v>64</ns0:v>
+      </ns0:c>
+      <ns0:c r="D25" s="1" t="s">
+        <ns0:v>69</ns0:v>
+      </ns0:c>
+      <ns0:c r="E25" s="1" t="s">
+        <ns0:v>70</ns0:v>
+      </ns0:c>
+      <ns0:c r="G25" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A26" s="1" t="s">
+        <ns0:v>71</ns0:v>
+      </ns0:c>
+      <ns0:c r="B26" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C26" s="1" t="s">
+        <ns0:v>72</ns0:v>
+      </ns0:c>
+      <ns0:c r="D26" s="1" t="s">
+        <ns0:v>73</ns0:v>
+      </ns0:c>
+      <ns0:c r="E26" s="1" t="s">
+        <ns0:v>74</ns0:v>
+      </ns0:c>
+      <ns0:c r="G26" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A27" s="1" t="s">
+        <ns0:v>71</ns0:v>
+      </ns0:c>
+      <ns0:c r="B27" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C27" s="1" t="s">
+        <ns0:v>72</ns0:v>
+      </ns0:c>
+      <ns0:c r="D27" s="1" t="s">
+        <ns0:v>75</ns0:v>
+      </ns0:c>
+      <ns0:c r="E27" s="1" t="s">
+        <ns0:v>76</ns0:v>
+      </ns0:c>
+      <ns0:c r="G27" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A28" s="1" t="s">
+        <ns0:v>71</ns0:v>
+      </ns0:c>
+      <ns0:c r="B28" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C28" s="1" t="s">
+        <ns0:v>72</ns0:v>
+      </ns0:c>
+      <ns0:c r="D28" s="1" t="s">
+        <ns0:v>77</ns0:v>
+      </ns0:c>
+      <ns0:c r="E28" s="1" t="s">
+        <ns0:v>78</ns0:v>
+      </ns0:c>
+      <ns0:c r="G28" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A29" s="1" t="s">
+        <ns0:v>71</ns0:v>
+      </ns0:c>
+      <ns0:c r="B29" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C29" s="1" t="s">
+        <ns0:v>79</ns0:v>
+      </ns0:c>
+      <ns0:c r="D29" s="1" t="s">
+        <ns0:v>80</ns0:v>
+      </ns0:c>
+      <ns0:c r="E29" s="1" t="s">
+        <ns0:v>81</ns0:v>
+      </ns0:c>
+      <ns0:c r="G29" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A30" s="1" t="s">
+        <ns0:v>71</ns0:v>
+      </ns0:c>
+      <ns0:c r="B30" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C30" s="1" t="s">
+        <ns0:v>79</ns0:v>
+      </ns0:c>
+      <ns0:c r="D30" s="1" t="s">
+        <ns0:v>82</ns0:v>
+      </ns0:c>
+      <ns0:c r="E30" s="1" t="s">
+        <ns0:v>83</ns0:v>
+      </ns0:c>
+      <ns0:c r="G30" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A31" s="1" t="s">
+        <ns0:v>71</ns0:v>
+      </ns0:c>
+      <ns0:c r="B31" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C31" s="1" t="s">
+        <ns0:v>79</ns0:v>
+      </ns0:c>
+      <ns0:c r="D31" s="1" t="s">
+        <ns0:v>84</ns0:v>
+      </ns0:c>
+      <ns0:c r="E31" s="1" t="s">
+        <ns0:v>85</ns0:v>
+      </ns0:c>
+      <ns0:c r="G31" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A32" s="1" t="s">
+        <ns0:v>86</ns0:v>
+      </ns0:c>
+      <ns0:c r="B32" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C32" s="1" t="s">
+        <ns0:v>87</ns0:v>
+      </ns0:c>
+      <ns0:c r="D32" s="1" t="s">
+        <ns0:v>88</ns0:v>
+      </ns0:c>
+      <ns0:c r="E32" s="1" t="s">
+        <ns0:v>89</ns0:v>
+      </ns0:c>
+      <ns0:c r="G32" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A33" s="1" t="s">
+        <ns0:v>86</ns0:v>
+      </ns0:c>
+      <ns0:c r="B33" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C33" s="1" t="s">
+        <ns0:v>87</ns0:v>
+      </ns0:c>
+      <ns0:c r="D33" s="1" t="s">
+        <ns0:v>90</ns0:v>
+      </ns0:c>
+      <ns0:c r="E33" s="1" t="s">
+        <ns0:v>91</ns0:v>
+      </ns0:c>
+      <ns0:c r="G33" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A34" s="1" t="s">
+        <ns0:v>86</ns0:v>
+      </ns0:c>
+      <ns0:c r="B34" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C34" s="1" t="s">
+        <ns0:v>87</ns0:v>
+      </ns0:c>
+      <ns0:c r="D34" s="1" t="s">
+        <ns0:v>92</ns0:v>
+      </ns0:c>
+      <ns0:c r="E34" s="1" t="s">
+        <ns0:v>93</ns0:v>
+      </ns0:c>
+      <ns0:c r="G34" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A35" s="1" t="s">
+        <ns0:v>86</ns0:v>
+      </ns0:c>
+      <ns0:c r="B35" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C35" s="1" t="s">
+        <ns0:v>94</ns0:v>
+      </ns0:c>
+      <ns0:c r="D35" s="1" t="s">
+        <ns0:v>95</ns0:v>
+      </ns0:c>
+      <ns0:c r="E35" s="1" t="s">
+        <ns0:v>96</ns0:v>
+      </ns0:c>
+      <ns0:c r="G35" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A36" s="1" t="s">
+        <ns0:v>86</ns0:v>
+      </ns0:c>
+      <ns0:c r="B36" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C36" s="1" t="s">
+        <ns0:v>94</ns0:v>
+      </ns0:c>
+      <ns0:c r="D36" s="1" t="s">
+        <ns0:v>97</ns0:v>
+      </ns0:c>
+      <ns0:c r="E36" s="1" t="s">
+        <ns0:v>98</ns0:v>
+      </ns0:c>
+      <ns0:c r="G36" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A37" s="1" t="s">
+        <ns0:v>86</ns0:v>
+      </ns0:c>
+      <ns0:c r="B37" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C37" s="1" t="s">
+        <ns0:v>94</ns0:v>
+      </ns0:c>
+      <ns0:c r="D37" s="1" t="s">
+        <ns0:v>99</ns0:v>
+      </ns0:c>
+      <ns0:c r="E37" s="1" t="s">
+        <ns0:v>100</ns0:v>
+      </ns0:c>
+      <ns0:c r="G37" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A38" s="1" t="s">
+        <ns0:v>101</ns0:v>
+      </ns0:c>
+      <ns0:c r="B38" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C38" s="1" t="s">
+        <ns0:v>102</ns0:v>
+      </ns0:c>
+      <ns0:c r="D38" s="1" t="s">
+        <ns0:v>103</ns0:v>
+      </ns0:c>
+      <ns0:c r="E38" s="1" t="s">
+        <ns0:v>104</ns0:v>
+      </ns0:c>
+      <ns0:c r="G38" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A39" s="1" t="s">
+        <ns0:v>101</ns0:v>
+      </ns0:c>
+      <ns0:c r="B39" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C39" s="1" t="s">
+        <ns0:v>102</ns0:v>
+      </ns0:c>
+      <ns0:c r="D39" s="1" t="s">
+        <ns0:v>105</ns0:v>
+      </ns0:c>
+      <ns0:c r="E39" s="1" t="s">
+        <ns0:v>106</ns0:v>
+      </ns0:c>
+      <ns0:c r="G39" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A40" s="1" t="s">
+        <ns0:v>101</ns0:v>
+      </ns0:c>
+      <ns0:c r="B40" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C40" s="1" t="s">
+        <ns0:v>102</ns0:v>
+      </ns0:c>
+      <ns0:c r="D40" s="1" t="s">
+        <ns0:v>107</ns0:v>
+      </ns0:c>
+      <ns0:c r="E40" s="1" t="s">
+        <ns0:v>108</ns0:v>
+      </ns0:c>
+      <ns0:c r="G40" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A41" s="1" t="s">
+        <ns0:v>101</ns0:v>
+      </ns0:c>
+      <ns0:c r="B41" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C41" s="1" t="s">
+        <ns0:v>109</ns0:v>
+      </ns0:c>
+      <ns0:c r="D41" s="1" t="s">
+        <ns0:v>110</ns0:v>
+      </ns0:c>
+      <ns0:c r="E41" s="1" t="s">
+        <ns0:v>111</ns0:v>
+      </ns0:c>
+      <ns0:c r="G41" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A42" s="1" t="s">
+        <ns0:v>101</ns0:v>
+      </ns0:c>
+      <ns0:c r="B42" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C42" s="1" t="s">
+        <ns0:v>109</ns0:v>
+      </ns0:c>
+      <ns0:c r="D42" s="1" t="s">
+        <ns0:v>112</ns0:v>
+      </ns0:c>
+      <ns0:c r="E42" s="1" t="s">
+        <ns0:v>113</ns0:v>
+      </ns0:c>
+      <ns0:c r="G42" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A43" s="1" t="s">
+        <ns0:v>101</ns0:v>
+      </ns0:c>
+      <ns0:c r="B43" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C43" s="1" t="s">
+        <ns0:v>109</ns0:v>
+      </ns0:c>
+      <ns0:c r="D43" s="1" t="s">
+        <ns0:v>114</ns0:v>
+      </ns0:c>
+      <ns0:c r="E43" s="1" t="s">
+        <ns0:v>115</ns0:v>
+      </ns0:c>
+      <ns0:c r="G43" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A44" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B44" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C44" s="1" t="s">
+        <ns0:v>117</ns0:v>
+      </ns0:c>
+      <ns0:c r="D44" s="1" t="s">
+        <ns0:v>118</ns0:v>
+      </ns0:c>
+      <ns0:c r="E44" s="1" t="s">
+        <ns0:v>119</ns0:v>
+      </ns0:c>
+      <ns0:c r="G44" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A45" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B45" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C45" s="1" t="s">
+        <ns0:v>117</ns0:v>
+      </ns0:c>
+      <ns0:c r="D45" s="1" t="s">
+        <ns0:v>120</ns0:v>
+      </ns0:c>
+      <ns0:c r="E45" s="1" t="s">
+        <ns0:v>121</ns0:v>
+      </ns0:c>
+      <ns0:c r="G45" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A46" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B46" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C46" s="1" t="s">
+        <ns0:v>117</ns0:v>
+      </ns0:c>
+      <ns0:c r="D46" s="1" t="s">
+        <ns0:v>122</ns0:v>
+      </ns0:c>
+      <ns0:c r="E46" s="1" t="s">
+        <ns0:v>123</ns0:v>
+      </ns0:c>
+      <ns0:c r="G46" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A47" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B47" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C47" s="1" t="s">
+        <ns0:v>124</ns0:v>
+      </ns0:c>
+      <ns0:c r="D47" s="1" t="s">
+        <ns0:v>125</ns0:v>
+      </ns0:c>
+      <ns0:c r="E47" s="1" t="s">
+        <ns0:v>126</ns0:v>
+      </ns0:c>
+      <ns0:c r="G47" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A48" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B48" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C48" s="1" t="s">
+        <ns0:v>124</ns0:v>
+      </ns0:c>
+      <ns0:c r="D48" s="1" t="s">
+        <ns0:v>127</ns0:v>
+      </ns0:c>
+      <ns0:c r="E48" s="1" t="s">
+        <ns0:v>128</ns0:v>
+      </ns0:c>
+      <ns0:c r="G48" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A49" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B49" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C49" s="1" t="s">
+        <ns0:v>124</ns0:v>
+      </ns0:c>
+      <ns0:c r="D49" s="1" t="s">
+        <ns0:v>129</ns0:v>
+      </ns0:c>
+      <ns0:c r="E49" s="1" t="s">
+        <ns0:v>130</ns0:v>
+      </ns0:c>
+      <ns0:c r="G49" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="50" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A50" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B50" s="1" t="s">
+        <ns0:v>28</ns0:v>
+      </ns0:c>
+      <ns0:c r="C50" s="1" t="s">
+        <ns0:v>131</ns0:v>
+      </ns0:c>
+      <ns0:c r="D50" s="1" t="s">
+        <ns0:v>132</ns0:v>
+      </ns0:c>
+      <ns0:c r="E50" s="1" t="s">
+        <ns0:v>133</ns0:v>
+      </ns0:c>
+      <ns0:c r="G50" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A51" s="1" t="s">
+        <ns0:v>116</ns0:v>
+      </ns0:c>
+      <ns0:c r="B51" s="1" t="s">
+        <ns0:v>28</ns0:v>
+      </ns0:c>
+      <ns0:c r="C51" s="1" t="s">
+        <ns0:v>131</ns0:v>
+      </ns0:c>
+      <ns0:c r="D51" s="1" t="s">
+        <ns0:v>134</ns0:v>
+      </ns0:c>
+      <ns0:c r="E51" s="1" t="s">
+        <ns0:v>135</ns0:v>
+      </ns0:c>
+      <ns0:c r="G51" s="1" t="s">
+        <ns0:v>51</ns0:v>
+      </ns0:c>
+    </ns0:row>
+  </ns0:sheetData>
+  <ns0:printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <ns0:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <ns0:pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <ns0:headerFooter differentFirst="false" differentOddEven="false">
+    <ns0:oddHeader/>
+    <ns0:oddFooter/>
+  </ns0:headerFooter>
+</ns0:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<ns0:worksheet xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <ns0:sheetPr filterMode="false">
+    <ns0:pageSetUpPr fitToPage="false"/>
+  </ns0:sheetPr>
+  <ns0:dimension ref="A1:H51"/>
+  <ns0:sheetViews>
+    <ns0:sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <ns0:selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    </ns0:sheetView>
+  </ns0:sheetViews>
+  <ns0:sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <ns0:cols>
+    <ns0:col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.68"/>
+    <ns0:col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="60.79"/>
+    <ns0:col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.33"/>
+    <ns0:col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="97.79"/>
+    <ns0:col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="63.58"/>
+    <ns0:col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.33"/>
+    <ns0:col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="59.26"/>
+    <ns0:col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="1" width="8.68"/>
+  </ns0:cols>
+  <ns0:sheetData>
+    <ns0:row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A1" s="2" t="s">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+      <ns0:c r="B1" s="2" t="s">
+        <ns0:v>1</ns0:v>
+      </ns0:c>
+      <ns0:c r="C1" s="2" t="s">
+        <ns0:v>2</ns0:v>
+      </ns0:c>
+      <ns0:c r="D1" s="2" t="s">
+        <ns0:v>3</ns0:v>
+      </ns0:c>
+      <ns0:c r="E1" s="2" t="s">
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="F1" s="2" t="s">
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="G1" s="2" t="s">
+        <ns0:v>6</ns0:v>
+      </ns0:c>
+      <ns0:c r="H1" s="2" t="s">
+        <ns0:v>7</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A2" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B2" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C2" s="1" t="s">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="D2" s="1" t="s">
+        <ns0:v>11</ns0:v>
+      </ns0:c>
+      <ns0:c r="E2" s="1" t="s">
+        <ns0:v>12</ns0:v>
+      </ns0:c>
+      <ns0:c r="G2" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F2" s="1" t="s">
+        <ns0:v>136</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A3" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B3" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C3" s="1" t="s">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="D3" s="1" t="s">
+        <ns0:v>14</ns0:v>
+      </ns0:c>
+      <ns0:c r="E3" s="1" t="s">
+        <ns0:v>15</ns0:v>
+      </ns0:c>
+      <ns0:c r="G3" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F3" s="1" t="s">
+        <ns0:v>137</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A4" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B4" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C4" s="1" t="s">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="D4" s="1" t="s">
+        <ns0:v>16</ns0:v>
+      </ns0:c>
+      <ns0:c r="E4" s="1" t="s">
+        <ns0:v>17</ns0:v>
+      </ns0:c>
+      <ns0:c r="G4" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F4" s="1" t="s">
+        <ns0:v>138</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A5" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B5" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C5" s="1" t="s">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="D5" s="1" t="s">
+        <ns0:v>18</ns0:v>
+      </ns0:c>
+      <ns0:c r="E5" s="1" t="s">
+        <ns0:v>19</ns0:v>
+      </ns0:c>
+      <ns0:c r="G5" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F5" s="1" t="s">
+        <ns0:v>139</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A6" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B6" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C6" s="1" t="s">
+        <ns0:v>21</ns0:v>
+      </ns0:c>
+      <ns0:c r="D6" s="1" t="s">
+        <ns0:v>22</ns0:v>
+      </ns0:c>
+      <ns0:c r="E6" s="1" t="s">
+        <ns0:v>23</ns0:v>
+      </ns0:c>
+      <ns0:c r="G6" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F6" s="1" t="s">
+        <ns0:v>140</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A7" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B7" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C7" s="1" t="s">
+        <ns0:v>21</ns0:v>
+      </ns0:c>
+      <ns0:c r="D7" s="1" t="s">
+        <ns0:v>24</ns0:v>
+      </ns0:c>
+      <ns0:c r="E7" s="1" t="s">
+        <ns0:v>25</ns0:v>
+      </ns0:c>
+      <ns0:c r="G7" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F7" s="1" t="s">
+        <ns0:v>141</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A8" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B8" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C8" s="1" t="s">
+        <ns0:v>21</ns0:v>
+      </ns0:c>
+      <ns0:c r="D8" s="1" t="s">
+        <ns0:v>26</ns0:v>
+      </ns0:c>
+      <ns0:c r="E8" s="1" t="s">
+        <ns0:v>27</ns0:v>
+      </ns0:c>
+      <ns0:c r="G8" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F8" s="1" t="s">
+        <ns0:v>142</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A9" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B9" s="1" t="s">
+        <ns0:v>28</ns0:v>
+      </ns0:c>
+      <ns0:c r="C9" s="1" t="s">
+        <ns0:v>29</ns0:v>
+      </ns0:c>
+      <ns0:c r="D9" s="1" t="s">
+        <ns0:v>30</ns0:v>
+      </ns0:c>
+      <ns0:c r="E9" s="1" t="s">
+        <ns0:v>31</ns0:v>
+      </ns0:c>
+      <ns0:c r="G9" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F9" s="1" t="s">
+        <ns0:v>143</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A10" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B10" s="1" t="s">
+        <ns0:v>28</ns0:v>
+      </ns0:c>
+      <ns0:c r="C10" s="1" t="s">
+        <ns0:v>29</ns0:v>
+      </ns0:c>
+      <ns0:c r="D10" s="1" t="s">
+        <ns0:v>32</ns0:v>
+      </ns0:c>
+      <ns0:c r="E10" s="1" t="s">
+        <ns0:v>33</ns0:v>
+      </ns0:c>
+      <ns0:c r="G10" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F10" s="1" t="s">
+        <ns0:v>144</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A11" s="1" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="B11" s="1" t="s">
+        <ns0:v>28</ns0:v>
+      </ns0:c>
+      <ns0:c r="C11" s="1" t="s">
+        <ns0:v>29</ns0:v>
+      </ns0:c>
+      <ns0:c r="D11" s="1" t="s">
+        <ns0:v>34</ns0:v>
+      </ns0:c>
+      <ns0:c r="E11" s="1" t="s">
+        <ns0:v>35</ns0:v>
+      </ns0:c>
+      <ns0:c r="G11" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F11" s="1" t="s">
+        <ns0:v>145</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A12" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B12" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C12" s="1" t="s">
+        <ns0:v>37</ns0:v>
+      </ns0:c>
+      <ns0:c r="D12" s="1" t="s">
+        <ns0:v>38</ns0:v>
+      </ns0:c>
+      <ns0:c r="E12" s="1" t="s">
+        <ns0:v>39</ns0:v>
+      </ns0:c>
+      <ns0:c r="G12" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F12" s="1" t="s">
+        <ns0:v>146</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A13" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B13" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C13" s="1" t="s">
+        <ns0:v>37</ns0:v>
+      </ns0:c>
+      <ns0:c r="D13" s="1" t="s">
+        <ns0:v>40</ns0:v>
+      </ns0:c>
+      <ns0:c r="E13" s="1" t="s">
+        <ns0:v>41</ns0:v>
+      </ns0:c>
+      <ns0:c r="G13" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F13" s="1" t="s">
+        <ns0:v>147</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A14" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B14" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C14" s="1" t="s">
+        <ns0:v>37</ns0:v>
+      </ns0:c>
+      <ns0:c r="D14" s="1" t="s">
+        <ns0:v>42</ns0:v>
+      </ns0:c>
+      <ns0:c r="E14" s="1" t="s">
+        <ns0:v>43</ns0:v>
+      </ns0:c>
+      <ns0:c r="G14" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F14" s="1" t="s">
+        <ns0:v>148</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A15" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B15" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C15" s="1" t="s">
+        <ns0:v>37</ns0:v>
+      </ns0:c>
+      <ns0:c r="D15" s="1" t="s">
+        <ns0:v>44</ns0:v>
+      </ns0:c>
+      <ns0:c r="E15" s="1" t="s">
+        <ns0:v>45</ns0:v>
+      </ns0:c>
+      <ns0:c r="G15" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F15" s="1" t="s">
+        <ns0:v>149</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A16" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B16" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C16" s="1" t="s">
+        <ns0:v>37</ns0:v>
+      </ns0:c>
+      <ns0:c r="D16" s="1" t="s">
+        <ns0:v>46</ns0:v>
+      </ns0:c>
+      <ns0:c r="E16" s="1" t="s">
+        <ns0:v>47</ns0:v>
+      </ns0:c>
+      <ns0:c r="G16" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F16" s="1" t="s">
+        <ns0:v>150</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A17" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B17" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C17" s="1" t="s">
+        <ns0:v>48</ns0:v>
+      </ns0:c>
+      <ns0:c r="D17" s="1" t="s">
+        <ns0:v>49</ns0:v>
+      </ns0:c>
+      <ns0:c r="E17" s="1" t="s">
+        <ns0:v>50</ns0:v>
+      </ns0:c>
+      <ns0:c r="G17" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F17" s="1" t="s">
+        <ns0:v>151</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A18" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B18" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C18" s="1" t="s">
+        <ns0:v>48</ns0:v>
+      </ns0:c>
+      <ns0:c r="D18" s="1" t="s">
+        <ns0:v>52</ns0:v>
+      </ns0:c>
+      <ns0:c r="E18" s="1" t="s">
+        <ns0:v>53</ns0:v>
+      </ns0:c>
+      <ns0:c r="G18" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F18" s="1" t="s">
+        <ns0:v>152</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A19" s="1" t="s">
+        <ns0:v>36</ns0:v>
+      </ns0:c>
+      <ns0:c r="B19" s="1" t="s">
+        <ns0:v>20</ns0:v>
+      </ns0:c>
+      <ns0:c r="C19" s="1" t="s">
+        <ns0:v>48</ns0:v>
+      </ns0:c>
+      <ns0:c r="D19" s="1" t="s">
+        <ns0:v>54</ns0:v>
+      </ns0:c>
+      <ns0:c r="E19" s="1" t="s">
+        <ns0:v>55</ns0:v>
+      </ns0:c>
+      <ns0:c r="G19" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F19" s="1" t="s">
+        <ns0:v>153</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A20" s="1" t="s">
+        <ns0:v>56</ns0:v>
+      </ns0:c>
+      <ns0:c r="B20" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C20" s="1" t="s">
+        <ns0:v>57</ns0:v>
+      </ns0:c>
+      <ns0:c r="D20" s="1" t="s">
+        <ns0:v>58</ns0:v>
+      </ns0:c>
+      <ns0:c r="E20" s="1" t="s">
+        <ns0:v>59</ns0:v>
+      </ns0:c>
+      <ns0:c r="G20" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F20" s="1" t="s">
+        <ns0:v>154</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A21" s="1" t="s">
+        <ns0:v>56</ns0:v>
+      </ns0:c>
+      <ns0:c r="B21" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C21" s="1" t="s">
+        <ns0:v>57</ns0:v>
+      </ns0:c>
+      <ns0:c r="D21" s="1" t="s">
+        <ns0:v>60</ns0:v>
+      </ns0:c>
+      <ns0:c r="E21" s="1" t="s">
+        <ns0:v>61</ns0:v>
+      </ns0:c>
+      <ns0:c r="G21" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F21" s="1" t="s">
+        <ns0:v>155</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <ns0:c r="A22" s="1" t="s">
+        <ns0:v>56</ns0:v>
+      </ns0:c>
+      <ns0:c r="B22" s="1" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C22" s="1" t="s">
+        <ns0:v>57</ns0:v>
+      </ns0:c>
+      <ns0:c r="D22" s="1" t="s">
+        <ns0:v>62</ns0:v>
+      </ns0:c>
+      <ns0:c r="E22" s="1" t="s">
+        <ns0:v>63</ns0:v>
+      </ns0:c>
+      <ns0:c r="G22" s="1" t="s">
+        <ns0:v>13</ns0:v>
+      </ns0:c>
+      <ns0:c r="F22" s="1" t="s">
+        <ns0:v>156</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
* S05/G01: Backtest results: persistence and metrics calculation * S05/G02: Backtest detail UI: equity chart, trades table, and parameters
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -1560,9 +1560,14 @@
           <t>Persist equity curve and trades from Backtrader runs into backtest_equity_points and backtest_trades tables.</t>
         </is>
       </c>
+      <c r="F32" s="0" t="inlineStr">
+        <is>
+          <t>backtest_equity_points and backtest_trades tables added; engine now returns equity_curve and trades which are persisted per backtest.</t>
+        </is>
+      </c>
       <c r="G32" s="3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -1592,9 +1597,14 @@
           <t>Compute key metrics (total return, max drawdown, win rate, average win/loss, trade count) and store in metrics_json.</t>
         </is>
       </c>
+      <c r="F33" s="0" t="inlineStr">
+        <is>
+          <t>BacktestService computes total_return, max_drawdown, trade_count, win_rate, avg_win, avg_loss and stores them in metrics_json.</t>
+        </is>
+      </c>
       <c r="G33" s="3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -1624,9 +1634,14 @@
           <t>Expose API endpoints to fetch backtest summary, equity series, and trades for a given backtest_id.</t>
         </is>
       </c>
+      <c r="F34" s="0" t="inlineStr">
+        <is>
+          <t>API exposes /api/backtests/{id}/equity and /api/backtests/{id}/trades for detailed results.</t>
+        </is>
+      </c>
       <c r="G34" s="3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -1656,9 +1671,14 @@
           <t>Implement Backtest detail page with summary metrics and equity curve chart (interactive).</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Backtests page now shows a Backtest Details panel with summary metrics and an equity curve chart for the selected run.</t>
+        </is>
+      </c>
       <c r="G35" s="3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -1688,9 +1708,14 @@
           <t>Add trades table with sorting/filtering, showing entry/exit, P&amp;L, and basic stats.</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Trades table added to Backtest Details panel, listing entry/exit, side, size, and PnL for each trade.</t>
+        </is>
+      </c>
       <c r="G36" s="3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -1720,9 +1745,14 @@
           <t>Optionally overlay buy/sell markers on price chart for one-symbol backtests.</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Backtest Details panel also shows the parameter set used (when available), with JSON rendered readably.</t>
+        </is>
+      </c>
       <c r="G37" s="3" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S06/G01: Backtest Overhaul: backend metrics and projections
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -365,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
@@ -384,1827 +384,2119 @@
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>sprint#</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>group#</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>group task description</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>task#</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="0" t="inlineStr">
         <is>
           <t>task description</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="0" t="inlineStr">
         <is>
           <t>remarks</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="G1" s="0" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="H1" s="6" t="inlineStr">
+      <c r="H1" s="0" t="inlineStr">
         <is>
           <t>deviations (from original plan)</t>
         </is>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" s="5">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>Backend foundation: FastAPI skeleton, config, meta DB setup</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>S01_G01_TB001</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="0" t="inlineStr">
         <is>
           <t>Create FastAPI project skeleton with basic app factory and routing structure.</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F2" s="0" t="inlineStr">
         <is>
           <t>FastAPI app factory and /health endpoint created.</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="G2" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="5">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>Backend foundation: FastAPI skeleton, config, meta DB setup</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>S01_G01_TB002</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="0" t="inlineStr">
         <is>
           <t>Implement configuration loader (env-based) for DB paths, Kite keys, and app settings.</t>
         </is>
       </c>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="F3" s="0" t="inlineStr">
         <is>
           <t>Env-based Settings config using pydantic-settings added.</t>
         </is>
       </c>
-      <c r="G3" s="4" t="inlineStr">
+      <c r="G3" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="4" ht="27.75" customHeight="1" s="5">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>Backend foundation: FastAPI skeleton, config, meta DB setup</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>S01_G01_TB003</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t>Design and create sigmaqlab_meta.db schema migration for core tables (strategies, strategy_parameters, backtests).</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
+      <c r="F4" s="0" t="inlineStr">
         <is>
           <t>sigmaqlab_meta.db schema for strategies/params/backtests wired via SQLAlchemy.</t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr">
+      <c r="G4" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>Backend foundation: FastAPI skeleton, config, meta DB setup</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>S01_G01_TB004</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>Set up structured logging for backend (JSON or key-value format) with log levels and request logging.</t>
         </is>
       </c>
-      <c r="F5" s="4" t="inlineStr">
+      <c r="F5" s="0" t="inlineStr">
         <is>
           <t>JSON logging with level/timestamp and Uvicorn integration configured.</t>
         </is>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="G5" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="5">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>Frontend foundation: React+TS+MUI scaffold and base layout</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>S01_G02_TF001</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="E6" s="0" t="inlineStr">
         <is>
           <t>Create React + TypeScript + Vite (or CRA) app and integrate Material UI.</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="F6" s="0" t="inlineStr">
         <is>
           <t>React + TS + Vite + MUI frontend scaffolded.</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="G6" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="5">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>Frontend foundation: React+TS+MUI scaffold and base layout</t>
         </is>
       </c>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>S01_G02_TF002</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E7" s="0" t="inlineStr">
         <is>
           <t>Implement global layout: AppBar with SigmaQLab branding, navigation skeleton, and basic dark theme.</t>
         </is>
       </c>
-      <c r="F7" s="4" t="inlineStr">
+      <c r="F7" s="0" t="inlineStr">
         <is>
           <t>Global dark theme and SigmaQLab layout (AppBar + nav) implemented.</t>
         </is>
       </c>
-      <c r="G7" s="4" t="inlineStr">
+      <c r="G7" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="8" ht="27.75" customHeight="1" s="5">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>Frontend foundation: React+TS+MUI scaffold and base layout</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>S01_G02_TF003</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
+      <c r="E8" s="0" t="inlineStr">
         <is>
           <t>Set up React Router with routes for Dashboard, Strategies, Backtests, Data, Settings.</t>
         </is>
       </c>
-      <c r="F8" s="4" t="inlineStr">
+      <c r="F8" s="0" t="inlineStr">
         <is>
           <t>React Router routes for Dashboard/Strategies/Backtests/Data/Settings added.</t>
         </is>
       </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="G8" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="5">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>Developer experience: tooling, linting, and pre-commit</t>
         </is>
       </c>
-      <c r="D9" s="4" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>S01_G03_TB001</t>
         </is>
       </c>
-      <c r="E9" s="4" t="inlineStr">
+      <c r="E9" s="0" t="inlineStr">
         <is>
           <t>Configure backend tooling: black, isort, mypy/ruff, and add pre-commit hooks.</t>
         </is>
       </c>
-      <c r="F9" s="4" t="inlineStr">
+      <c r="F9" s="0" t="inlineStr">
         <is>
           <t>Backend tooling (black, ruff, pytest, pre-commit) configured.</t>
         </is>
       </c>
-      <c r="G9" s="4" t="inlineStr">
+      <c r="G9" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="5">
-      <c r="A10" s="4" t="inlineStr">
+      <c r="A10" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>Developer experience: tooling, linting, and pre-commit</t>
         </is>
       </c>
-      <c r="D10" s="4" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>S01_G03_TF002</t>
         </is>
       </c>
-      <c r="E10" s="4" t="inlineStr">
+      <c r="E10" s="0" t="inlineStr">
         <is>
           <t>Configure frontend tooling: ESLint, Prettier, TypeScript strict settings.</t>
         </is>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="F10" s="0" t="inlineStr">
         <is>
           <t>Frontend tooling (ESLint, Prettier, strict TS) configured.</t>
         </is>
       </c>
-      <c r="G10" s="4" t="inlineStr">
+      <c r="G10" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="5">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="0" t="inlineStr">
         <is>
           <t>S01</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>Developer experience: tooling, linting, and pre-commit</t>
         </is>
       </c>
-      <c r="D11" s="4" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>S01_G03_TB003</t>
         </is>
       </c>
-      <c r="E11" s="4" t="inlineStr">
+      <c r="E11" s="0" t="inlineStr">
         <is>
           <t>Add basic test harness for backend (pytest) with one sample test to validate CI wiring.</t>
         </is>
       </c>
-      <c r="F11" s="4" t="inlineStr">
+      <c r="F11" s="0" t="inlineStr">
         <is>
           <t>Basic pytest harness with /health test in place.</t>
         </is>
       </c>
-      <c r="G11" s="4" t="inlineStr">
+      <c r="G11" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="5">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>Data service: Kite/yfinance integration and price DB persistence</t>
         </is>
       </c>
-      <c r="D12" s="4" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>S02_G01_TB001</t>
         </is>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="E12" s="0" t="inlineStr">
         <is>
           <t>Implement Zerodha Kite client wrapper for historical OHLCV and holdings (read-only).</t>
         </is>
       </c>
-      <c r="F12" s="4" t="inlineStr">
+      <c r="F12" s="0" t="inlineStr">
         <is>
           <t>Kite client wrapper for historical OHLCV implemented.</t>
         </is>
       </c>
-      <c r="G12" s="4" t="inlineStr">
+      <c r="G12" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="5">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C13" s="4" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>Data service: Kite/yfinance integration and price DB persistence</t>
         </is>
       </c>
-      <c r="D13" s="4" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>S02_G01_TB002</t>
         </is>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="0" t="inlineStr">
         <is>
           <t>Implement optional yfinance/CSV loader as fallback data provider.</t>
         </is>
       </c>
-      <c r="F13" s="4" t="inlineStr">
+      <c r="F13" s="0" t="inlineStr">
         <is>
           <t>yfinance and CSV data providers added as fallbacks.</t>
         </is>
       </c>
-      <c r="G13" s="4" t="inlineStr">
+      <c r="G13" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="5">
-      <c r="A14" s="4" t="inlineStr">
+      <c r="A14" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B14" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C14" s="4" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>Data service: Kite/yfinance integration and price DB persistence</t>
         </is>
       </c>
-      <c r="D14" s="4" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>S02_G01_TB003</t>
         </is>
       </c>
-      <c r="E14" s="4" t="inlineStr">
+      <c r="E14" s="0" t="inlineStr">
         <is>
           <t>Design and create sigmaqlab_prices.db schema (price_bars table with indices).</t>
         </is>
       </c>
-      <c r="F14" s="4" t="inlineStr">
+      <c r="F14" s="0" t="inlineStr">
         <is>
           <t>sigmaqlab_prices.db and price_bars schema created.</t>
         </is>
       </c>
-      <c r="G14" s="4" t="inlineStr">
+      <c r="G14" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="15" ht="27.75" customHeight="1" s="5">
-      <c r="A15" s="4" t="inlineStr">
+      <c r="A15" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C15" s="4" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>Data service: Kite/yfinance integration and price DB persistence</t>
         </is>
       </c>
-      <c r="D15" s="4" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>S02_G01_TB004</t>
         </is>
       </c>
-      <c r="E15" s="4" t="inlineStr">
+      <c r="E15" s="0" t="inlineStr">
         <is>
           <t>Implement Data Service functions to fetch, normalize, and persist OHLCV data from providers into price DB.</t>
         </is>
       </c>
-      <c r="F15" s="4" t="inlineStr">
+      <c r="F15" s="0" t="inlineStr">
         <is>
           <t>DataService to fetch/normalise/persist OHLCV into prices DB implemented.</t>
         </is>
       </c>
-      <c r="G15" s="4" t="inlineStr">
+      <c r="G15" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="5">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="A16" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>Data service: Kite/yfinance integration and price DB persistence</t>
         </is>
       </c>
-      <c r="D16" s="4" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>S02_G01_TB005</t>
         </is>
       </c>
-      <c r="E16" s="4" t="inlineStr">
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>Expose FastAPI endpoint to trigger data fetch for given symbol, timeframe, and date range.</t>
         </is>
       </c>
-      <c r="F16" s="4" t="inlineStr">
+      <c r="F16" s="0" t="inlineStr">
         <is>
           <t>/api/data/fetch endpoint added and covered by tests.</t>
         </is>
       </c>
-      <c r="G16" s="4" t="inlineStr">
+      <c r="G16" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="5">
-      <c r="A17" s="4" t="inlineStr">
+      <c r="A17" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B17" s="4" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C17" s="4" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>Data management UI: fetch, list, and preview data</t>
         </is>
       </c>
-      <c r="D17" s="4" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>S02_G02_TF001</t>
         </is>
       </c>
-      <c r="E17" s="4" t="inlineStr">
+      <c r="E17" s="0" t="inlineStr">
         <is>
           <t>Create Data page with form to trigger data fetch via API (symbol, timeframe, date range).</t>
         </is>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="F17" s="0" t="inlineStr">
         <is>
           <t>Data page fetch form wired to backend data fetch API.</t>
         </is>
       </c>
-      <c r="G17" s="4" t="inlineStr">
+      <c r="G17" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="18" ht="27.75" customHeight="1" s="5">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C18" s="4" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>Data management UI: fetch, list, and preview data</t>
         </is>
       </c>
-      <c r="D18" s="4" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>S02_G02_TF002</t>
         </is>
       </c>
-      <c r="E18" s="4" t="inlineStr">
+      <c r="E18" s="0" t="inlineStr">
         <is>
           <t>Implement table listing available symbol/timeframe combinations and coverage ranges.</t>
         </is>
       </c>
-      <c r="F18" s="4" t="inlineStr">
+      <c r="F18" s="0" t="inlineStr">
         <is>
           <t>Coverage summary table with source column, row selection, Select All, and Delete Selected controls.</t>
         </is>
       </c>
-      <c r="G18" s="4" t="inlineStr">
+      <c r="G18" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="19" ht="41.75" customHeight="1" s="5">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" s="0" t="inlineStr">
         <is>
           <t>S02</t>
         </is>
       </c>
-      <c r="B19" s="4" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>Data management UI: fetch, list, and preview data</t>
         </is>
       </c>
-      <c r="D19" s="4" t="inlineStr">
+      <c r="D19" s="0" t="inlineStr">
         <is>
           <t>S02_G02_TF003</t>
         </is>
       </c>
-      <c r="E19" s="4" t="inlineStr">
+      <c r="E19" s="0" t="inlineStr">
         <is>
           <t>Add simple price &amp; volume preview chart for selected symbol/timeframe using chosen charting library.</t>
         </is>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="F19" s="0" t="inlineStr">
         <is>
           <t>Preview now uses lightweight-charts with grouped indicator toggles, tall adjustable chart, volume bars toggle, range presets (intraday + calendar), simple tools (last price line/latest-bar marker), and synced price/oscillator panes.</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr">
+      <c r="G19" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="5">
-      <c r="A20" s="4" t="inlineStr">
+      <c r="A20" s="0" t="inlineStr">
         <is>
           <t>S03</t>
         </is>
       </c>
-      <c r="B20" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C20" s="4" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>Strategy service: metadata and parameter storage</t>
         </is>
       </c>
-      <c r="D20" s="4" t="inlineStr">
+      <c r="D20" s="0" t="inlineStr">
         <is>
           <t>S03_G01_TB001</t>
         </is>
       </c>
-      <c r="E20" s="4" t="inlineStr">
+      <c r="E20" s="0" t="inlineStr">
         <is>
           <t>Implement Strategy CRUD endpoints (create, list, get, update, delete) in FastAPI.</t>
         </is>
       </c>
-      <c r="F20" s="4" t="inlineStr">
+      <c r="F20" s="0" t="inlineStr">
         <is>
           <t>Strategy CRUD API endpoints implemented.</t>
         </is>
       </c>
-      <c r="G20" s="4" t="inlineStr">
+      <c r="G20" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="5">
-      <c r="A21" s="4" t="inlineStr">
+      <c r="A21" s="0" t="inlineStr">
         <is>
           <t>S03</t>
         </is>
       </c>
-      <c r="B21" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C21" s="4" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>Strategy service: metadata and parameter storage</t>
         </is>
       </c>
-      <c r="D21" s="4" t="inlineStr">
+      <c r="D21" s="0" t="inlineStr">
         <is>
           <t>S03_G01_TB002</t>
         </is>
       </c>
-      <c r="E21" s="4" t="inlineStr">
+      <c r="E21" s="0" t="inlineStr">
         <is>
           <t>Implement Strategy Parameters CRUD endpoints and tie them to strategies.</t>
         </is>
       </c>
-      <c r="F21" s="4" t="inlineStr">
+      <c r="F21" s="0" t="inlineStr">
         <is>
           <t>Strategy parameter CRUD endpoints wired to strategies.</t>
         </is>
       </c>
-      <c r="G21" s="4" t="inlineStr">
+      <c r="G21" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="22" ht="41.75" customHeight="1" s="5">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="A22" s="0" t="inlineStr">
         <is>
           <t>S03</t>
         </is>
       </c>
-      <c r="B22" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C22" s="4" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>Strategy service: metadata and parameter storage</t>
         </is>
       </c>
-      <c r="D22" s="4" t="inlineStr">
+      <c r="D22" s="0" t="inlineStr">
         <is>
           <t>S03_G01_TB003</t>
         </is>
       </c>
-      <c r="E22" s="4" t="inlineStr">
+      <c r="E22" s="0" t="inlineStr">
         <is>
           <t>Add fields for tags, categories, statuses, and integration metadata in schema and API models.</t>
         </is>
       </c>
-      <c r="F22" s="4" t="inlineStr">
+      <c r="F22" s="0" t="inlineStr">
         <is>
           <t>Tags/category/status/integration fields exposed in API models. Engine code field added to Strategy schema and API models so multiple business codes can share one engine implementation.</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr">
+      <c r="G22" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="23" ht="41.75" customHeight="1" s="5">
-      <c r="A23" s="4" t="inlineStr">
+      <c r="A23" s="0" t="inlineStr">
         <is>
           <t>S03</t>
         </is>
       </c>
-      <c r="B23" s="4" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C23" s="4" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>Strategy Library UI: list, details, and parameter sets</t>
         </is>
       </c>
-      <c r="D23" s="4" t="inlineStr">
+      <c r="D23" s="0" t="inlineStr">
         <is>
           <t>S03_G02_TF001</t>
         </is>
       </c>
-      <c r="E23" s="4" t="inlineStr">
+      <c r="E23" s="0" t="inlineStr">
         <is>
           <t>Implement Strategies list view with filters (status, category, search) and pagination.</t>
         </is>
       </c>
-      <c r="F23" s="4" t="inlineStr">
+      <c r="F23" s="0" t="inlineStr">
         <is>
           <t>Strategy list view in React (table) with edit/delete implemented. Strategies list shows engine implementation and supports filtering by engine_code.</t>
         </is>
       </c>
-      <c r="G23" s="4" t="inlineStr">
+      <c r="G23" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="5">
-      <c r="A24" s="4" t="inlineStr">
+      <c r="A24" s="0" t="inlineStr">
         <is>
           <t>S03</t>
         </is>
       </c>
-      <c r="B24" s="4" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>Strategy Library UI: list, details, and parameter sets</t>
         </is>
       </c>
-      <c r="D24" s="4" t="inlineStr">
+      <c r="D24" s="0" t="inlineStr">
         <is>
           <t>S03_G02_TF002</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr">
+      <c r="E24" s="0" t="inlineStr">
         <is>
           <t>Implement Strategy detail view showing description, tags, and recent backtests placeholder.</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
+      <c r="F24" s="0" t="inlineStr">
         <is>
           <t>Strategy detail panel with status/tags/integration fields added.</t>
         </is>
       </c>
-      <c r="G24" s="4" t="inlineStr">
+      <c r="G24" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="5">
-      <c r="A25" s="4" t="inlineStr">
+      <c r="A25" s="0" t="inlineStr">
         <is>
           <t>S03</t>
         </is>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C25" s="4" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>Strategy Library UI: list, details, and parameter sets</t>
         </is>
       </c>
-      <c r="D25" s="4" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>S03_G02_TF003</t>
         </is>
       </c>
-      <c r="E25" s="4" t="inlineStr">
+      <c r="E25" s="0" t="inlineStr">
         <is>
           <t>Add parameter set management UI (list, create, edit, delete) for each strategy.</t>
         </is>
       </c>
-      <c r="F25" s="4" t="inlineStr">
+      <c r="F25" s="0" t="inlineStr">
         <is>
           <t>Parameter sets table and JSON-based create/edit/delete wired to API.</t>
         </is>
       </c>
-      <c r="G25" s="4" t="inlineStr">
+      <c r="G25" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="26" ht="41.75" customHeight="1" s="5">
-      <c r="A26" s="4" t="inlineStr">
+      <c r="A26" s="0" t="inlineStr">
         <is>
           <t>S04</t>
         </is>
       </c>
-      <c r="B26" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C26" s="4" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>Backtest engine: Backtrader integration and engine interface</t>
         </is>
       </c>
-      <c r="D26" s="4" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>S04_G01_TB001</t>
         </is>
       </c>
-      <c r="E26" s="4" t="inlineStr">
+      <c r="E26" s="0" t="inlineStr">
         <is>
           <t>Define Strategy Engine interface and BacktestResult data models in backend.</t>
         </is>
       </c>
-      <c r="F26" s="4" t="inlineStr">
+      <c r="F26" s="0" t="inlineStr">
         <is>
           <t>BacktestConfig/BacktestResult engine interface and types defined. Backtest engine registry now keyed by engine_code (e.g. SmaCrossStrategy) with aliases for SMA_X* codes.</t>
         </is>
       </c>
-      <c r="G26" s="4" t="inlineStr">
+      <c r="G26" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="5">
-      <c r="A27" s="4" t="inlineStr">
+      <c r="A27" s="0" t="inlineStr">
         <is>
           <t>S04</t>
         </is>
       </c>
-      <c r="B27" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C27" s="4" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>Backtest engine: Backtrader integration and engine interface</t>
         </is>
       </c>
-      <c r="D27" s="4" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>S04_G01_TB002</t>
         </is>
       </c>
-      <c r="E27" s="4" t="inlineStr">
+      <c r="E27" s="0" t="inlineStr">
         <is>
           <t>Integrate Backtrader as primary engine and implement adapter that conforms to engine interface.</t>
         </is>
       </c>
-      <c r="F27" s="4" t="inlineStr">
+      <c r="F27" s="0" t="inlineStr">
         <is>
           <t>Backtrader engine (SMA_X) integrated behind StrategyEngine interface.</t>
         </is>
       </c>
-      <c r="G27" s="4" t="inlineStr">
+      <c r="G27" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="28" ht="41.75" customHeight="1" s="5">
-      <c r="A28" s="4" t="inlineStr">
+      <c r="A28" s="0" t="inlineStr">
         <is>
           <t>S04</t>
         </is>
       </c>
-      <c r="B28" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C28" s="4" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>Backtest engine: Backtrader integration and engine interface</t>
         </is>
       </c>
-      <c r="D28" s="4" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>S04_G01_TB003</t>
         </is>
       </c>
-      <c r="E28" s="4" t="inlineStr">
+      <c r="E28" s="0" t="inlineStr">
         <is>
           <t>Implement one reference strategy in Backtrader (e.g., simple SMA crossover) wired to a Strategy record.</t>
         </is>
       </c>
-      <c r="F28" s="4" t="inlineStr">
+      <c r="F28" s="0" t="inlineStr">
         <is>
           <t>BacktestService runs engine using DB price_bars and persists Backtest rows. BacktestService now uses Strategy.engine_code (falling back to code) when selecting engine implementation.</t>
         </is>
       </c>
-      <c r="G28" s="4" t="inlineStr">
+      <c r="G28" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="29" ht="28.35" customHeight="1" s="5">
-      <c r="A29" s="4" t="inlineStr">
+      <c r="A29" s="0" t="inlineStr">
         <is>
           <t>S04</t>
         </is>
       </c>
-      <c r="B29" s="4" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C29" s="4" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>Backtest execution: API endpoint and simple UI trigger</t>
         </is>
       </c>
-      <c r="D29" s="4" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>S04_G02_TB001</t>
         </is>
       </c>
-      <c r="E29" s="4" t="inlineStr">
+      <c r="E29" s="0" t="inlineStr">
         <is>
           <t>Implement API to run a single backtest given strategy_id, params_id, symbols, timeframe, and date range.</t>
         </is>
       </c>
-      <c r="F29" s="4" t="inlineStr">
+      <c r="F29" s="0" t="inlineStr">
         <is>
           <t>POST /api/backtests endpoint wired to BacktestService and covered by tests.</t>
         </is>
       </c>
-      <c r="G29" s="4" t="inlineStr">
+      <c r="G29" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="30" ht="28.35" customHeight="1" s="5">
-      <c r="A30" s="4" t="inlineStr">
+      <c r="A30" s="0" t="inlineStr">
         <is>
           <t>S04</t>
         </is>
       </c>
-      <c r="B30" s="4" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C30" s="4" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>Backtest execution: API endpoint and simple UI trigger</t>
         </is>
       </c>
-      <c r="D30" s="4" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>S04_G02_TF002</t>
         </is>
       </c>
-      <c r="E30" s="4" t="inlineStr">
+      <c r="E30" s="0" t="inlineStr">
         <is>
           <t>Add 'Run Backtest' modal/dialog in Strategy detail view to configure and submit a backtest.</t>
         </is>
       </c>
-      <c r="F30" s="4" t="inlineStr">
+      <c r="F30" s="0" t="inlineStr">
         <is>
           <t>Run backtest configuration form implemented on Backtests page instead of a modal in Strategy details.</t>
         </is>
       </c>
-      <c r="G30" s="4" t="inlineStr">
-        <is>
-          <t>implemented</t>
-        </is>
-      </c>
-      <c r="H30" s="4" t="inlineStr">
+      <c r="G30" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H30" s="0" t="inlineStr">
         <is>
           <t>UI deviation: backtest configuration lives on /backtests page; a strategy-scoped modal can be added later if needed.</t>
         </is>
       </c>
     </row>
     <row r="31" ht="28.35" customHeight="1" s="5">
-      <c r="A31" s="4" t="inlineStr">
+      <c r="A31" s="0" t="inlineStr">
         <is>
           <t>S04</t>
         </is>
       </c>
-      <c r="B31" s="4" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C31" s="4" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>Backtest execution: API endpoint and simple UI trigger</t>
         </is>
       </c>
-      <c r="D31" s="4" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>S04_G02_TF003</t>
         </is>
       </c>
-      <c r="E31" s="4" t="inlineStr">
+      <c r="E31" s="0" t="inlineStr">
         <is>
           <t>Create basic Backtests list page showing submitted runs, status, and key summary fields.</t>
         </is>
       </c>
-      <c r="F31" s="4" t="inlineStr">
+      <c r="F31" s="0" t="inlineStr">
         <is>
           <t>Backtests page lists recent runs with strategy, symbol, timeframe, status, PnL, and final value.</t>
         </is>
       </c>
-      <c r="G31" s="4" t="inlineStr">
+      <c r="G31" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="32" ht="28.35" customHeight="1" s="5">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="A32" s="0" t="inlineStr">
         <is>
           <t>S05</t>
         </is>
       </c>
-      <c r="B32" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C32" s="4" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>Backtest results: persistence and metrics calculation</t>
         </is>
       </c>
-      <c r="D32" s="4" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>S05_G01_TB001</t>
         </is>
       </c>
-      <c r="E32" s="4" t="inlineStr">
+      <c r="E32" s="0" t="inlineStr">
         <is>
           <t>Persist equity curve and trades from Backtrader runs into backtest_equity_points and backtest_trades tables.</t>
         </is>
       </c>
-      <c r="F32" s="7" t="inlineStr">
+      <c r="F32" s="0" t="inlineStr">
         <is>
           <t>backtest_equity_points and backtest_trades tables added; engine now returns equity_curve and trades which are persisted per backtest.</t>
         </is>
       </c>
-      <c r="G32" s="4" t="inlineStr">
+      <c r="G32" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="33" ht="28.35" customHeight="1" s="5">
-      <c r="A33" s="4" t="inlineStr">
+      <c r="A33" s="0" t="inlineStr">
         <is>
           <t>S05</t>
         </is>
       </c>
-      <c r="B33" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C33" s="4" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>Backtest results: persistence and metrics calculation</t>
         </is>
       </c>
-      <c r="D33" s="4" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>S05_G01_TB002</t>
         </is>
       </c>
-      <c r="E33" s="4" t="inlineStr">
+      <c r="E33" s="0" t="inlineStr">
         <is>
           <t>Compute key metrics (total return, max drawdown, win rate, average win/loss, trade count) and store in metrics_json.</t>
         </is>
       </c>
-      <c r="F33" s="7" t="inlineStr">
+      <c r="F33" s="0" t="inlineStr">
         <is>
           <t>BacktestService computes total_return, max_drawdown, trade_count, win_rate, avg_win, avg_loss and stores them in metrics_json.</t>
         </is>
       </c>
-      <c r="G33" s="4" t="inlineStr">
+      <c r="G33" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="34" ht="28.35" customHeight="1" s="5">
-      <c r="A34" s="4" t="inlineStr">
+      <c r="A34" s="0" t="inlineStr">
         <is>
           <t>S05</t>
         </is>
       </c>
-      <c r="B34" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C34" s="4" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>Backtest results: persistence and metrics calculation</t>
         </is>
       </c>
-      <c r="D34" s="4" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>S05_G01_TB003</t>
         </is>
       </c>
-      <c r="E34" s="4" t="inlineStr">
+      <c r="E34" s="0" t="inlineStr">
         <is>
           <t>Expose API endpoints to fetch backtest summary, equity series, and trades for a given backtest_id.</t>
         </is>
       </c>
-      <c r="F34" s="7" t="inlineStr">
+      <c r="F34" s="0" t="inlineStr">
         <is>
           <t>API exposes /api/backtests/{id}/equity and /api/backtests/{id}/trades for detailed results.</t>
         </is>
       </c>
-      <c r="G34" s="4" t="inlineStr">
+      <c r="G34" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="35" ht="28.35" customHeight="1" s="5">
-      <c r="A35" s="4" t="inlineStr">
+      <c r="A35" s="0" t="inlineStr">
         <is>
           <t>S05</t>
         </is>
       </c>
-      <c r="B35" s="4" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C35" s="4" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>Backtest detail UI: equity chart, trades table, and parameters</t>
         </is>
       </c>
-      <c r="D35" s="4" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>S05_G02_TF001</t>
         </is>
       </c>
-      <c r="E35" s="4" t="inlineStr">
+      <c r="E35" s="0" t="inlineStr">
         <is>
           <t>Implement Backtest detail page with summary metrics and equity curve chart (interactive).</t>
         </is>
       </c>
-      <c r="F35" s="7" t="inlineStr">
+      <c r="F35" s="0" t="inlineStr">
         <is>
           <t>Backtests page now shows a Backtest Details panel with summary metrics and an equity curve chart for the selected run.</t>
         </is>
       </c>
-      <c r="G35" s="4" t="inlineStr">
+      <c r="G35" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="36" ht="28.35" customHeight="1" s="5">
-      <c r="A36" s="4" t="inlineStr">
+      <c r="A36" s="0" t="inlineStr">
         <is>
           <t>S05</t>
         </is>
       </c>
-      <c r="B36" s="4" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C36" s="4" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>Backtest detail UI: equity chart, trades table, and parameters</t>
         </is>
       </c>
-      <c r="D36" s="4" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>S05_G02_TF002</t>
         </is>
       </c>
-      <c r="E36" s="4" t="inlineStr">
+      <c r="E36" s="0" t="inlineStr">
         <is>
           <t>Add trades table with sorting/filtering, showing entry/exit, P&amp;L, and basic stats.</t>
         </is>
       </c>
-      <c r="F36" s="7" t="inlineStr">
+      <c r="F36" s="0" t="inlineStr">
         <is>
           <t>Trades table added to Backtest Details panel, listing entry/exit, side, size, and PnL for each trade.</t>
         </is>
       </c>
-      <c r="G36" s="4" t="inlineStr">
+      <c r="G36" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="37" ht="28.35" customHeight="1" s="5">
-      <c r="A37" s="4" t="inlineStr">
+      <c r="A37" s="0" t="inlineStr">
         <is>
           <t>S05</t>
         </is>
       </c>
-      <c r="B37" s="4" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C37" s="4" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>Backtest detail UI: equity chart, trades table, and parameters</t>
         </is>
       </c>
-      <c r="D37" s="4" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>S05_G02_TF003</t>
         </is>
       </c>
-      <c r="E37" s="4" t="inlineStr">
+      <c r="E37" s="0" t="inlineStr">
         <is>
           <t>Optionally overlay buy/sell markers on price chart for one-symbol backtests.</t>
         </is>
       </c>
-      <c r="F37" s="7" t="inlineStr">
+      <c r="F37" s="0" t="inlineStr">
         <is>
           <t>Backtest Details panel also shows the parameter set used (when available), with JSON rendered readably.</t>
         </is>
       </c>
-      <c r="G37" s="4" t="inlineStr">
+      <c r="G37" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="5">
-      <c r="A38" s="4" t="inlineStr">
+      <c r="A38" s="0" t="inlineStr">
         <is>
           <t>S06</t>
         </is>
       </c>
-      <c r="B38" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C38" s="4" t="inlineStr">
-        <is>
-          <t>Batch backtesting: grid search and parallel execution</t>
-        </is>
-      </c>
-      <c r="D38" s="4" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: backend metrics and projections</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>S06_G01_TB001</t>
         </is>
       </c>
-      <c r="E38" s="4" t="inlineStr">
-        <is>
-          <t>Extend backtest API to accept parameter grids or multiple parameter sets for batch execution.</t>
-        </is>
-      </c>
-      <c r="G38" s="4" t="inlineStr">
+      <c r="E38" s="0" t="inlineStr">
+        <is>
+          <t>Extend Backtest model to store effective params, risk/cost/visualization configs, and richer metrics_json.</t>
+        </is>
+      </c>
+      <c r="F38" s="0" t="inlineStr">
+        <is>
+          <t>Backtest model extended with label/notes and JSON configs (params_effective/risk/costs/visual), plus migration helper.</t>
+        </is>
+      </c>
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1" s="5">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>S06</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: backend metrics and projections</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>S06_G01_TB002</t>
+        </is>
+      </c>
+      <c r="E39" s="0" t="inlineStr">
+        <is>
+          <t>Introduce backtest_trades and backtest_equity_points persistence (or equivalent) for trades and equity curves.</t>
+        </is>
+      </c>
+      <c r="F39" s="0" t="inlineStr">
+        <is>
+          <t>backtest_trades/backtest_equity_points persisted with extra per-trade metrics (pnl_pct, holding_period_bars, max_theoretical_pnl, capture ratio).</t>
+        </is>
+      </c>
+      <c r="G39" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="15" customHeight="1" s="5">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>S06</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: backend metrics and projections</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>S06_G01_TB003</t>
+        </is>
+      </c>
+      <c r="E40" s="0" t="inlineStr">
+        <is>
+          <t>Compute expanded backtest metrics (Sharpe, Sortino, alpha/beta, Calmar, volatility) from equity series.</t>
+        </is>
+      </c>
+      <c r="F40" s="0" t="inlineStr">
+        <is>
+          <t>Equity-based metrics (total_return, max_drawdown, volatility, Sharpe, Sortino, annual_return, Calmar) computed in BacktestService.</t>
+        </is>
+      </c>
+      <c r="G40" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="15" customHeight="1" s="5">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>S06</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: backend metrics and projections</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>S06_G01_TB004</t>
+        </is>
+      </c>
+      <c r="E41" s="0" t="inlineStr">
+        <is>
+          <t>Implement unrealised projection and per-trade what-if metrics using trades and price series.</t>
+        </is>
+      </c>
+      <c r="F41" s="0" t="inlineStr">
+        <is>
+          <t>Per-trade what-if metrics derived from price series and stored on BacktestTrade (what-if/max PnL and capture ratios).</t>
+        </is>
+      </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="15" customHeight="1" s="5">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>S06</t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: chart and series APIs</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>S06_G02_TB001</t>
+        </is>
+      </c>
+      <c r="E42" s="0" t="inlineStr">
+        <is>
+          <t>Add /api/backtests/{id}/chart-data endpoint returning price_bars, indicators, equity, projection, and trade markers.</t>
+        </is>
+      </c>
+      <c r="F42" s="0" t="inlineStr">
+        <is>
+          <t>JSON shape per qlab_bt_overhaul_prd.md 3.2.1.</t>
+        </is>
+      </c>
+      <c r="G42" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" s="5">
-      <c r="A39" s="4" t="inlineStr">
+    <row r="43" ht="15" customHeight="1" s="5">
+      <c r="A43" s="0" t="inlineStr">
         <is>
           <t>S06</t>
         </is>
       </c>
-      <c r="B39" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C39" s="4" t="inlineStr">
-        <is>
-          <t>Batch backtesting: grid search and parallel execution</t>
-        </is>
-      </c>
-      <c r="D39" s="4" t="inlineStr">
-        <is>
-          <t>S06_G01_TB002</t>
-        </is>
-      </c>
-      <c r="E39" s="4" t="inlineStr">
-        <is>
-          <t>Implement batch execution using ProcessPoolExecutor with isolation per run.</t>
-        </is>
-      </c>
-      <c r="G39" s="4" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: chart and series APIs</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>S06_G02_TB002</t>
+        </is>
+      </c>
+      <c r="E43" s="0" t="inlineStr">
+        <is>
+          <t>Add /api/backtests/{id}/trades endpoint returning enriched trade records with what-if metrics.</t>
+        </is>
+      </c>
+      <c r="F43" s="0" t="inlineStr">
+        <is>
+          <t>See qlab_bt_overhaul_prd.md 3.2.2.</t>
+        </is>
+      </c>
+      <c r="G43" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="40" ht="15" customHeight="1" s="5">
-      <c r="A40" s="4" t="inlineStr">
+    <row r="44" ht="15" customHeight="1" s="5">
+      <c r="A44" s="0" t="inlineStr">
         <is>
           <t>S06</t>
         </is>
       </c>
-      <c r="B40" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C40" s="4" t="inlineStr">
-        <is>
-          <t>Batch backtesting: grid search and parallel execution</t>
-        </is>
-      </c>
-      <c r="D40" s="4" t="inlineStr">
-        <is>
-          <t>S06_G01_TB003</t>
-        </is>
-      </c>
-      <c r="E40" s="4" t="inlineStr">
-        <is>
-          <t>Store batch group identifier to link multiple backtests that belong to one optimization run.</t>
-        </is>
-      </c>
-      <c r="G40" s="4" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: chart and series APIs</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>S06_G02_TB003</t>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t>Add /api/backtests/{id}/trades/export?format=csv endpoint for backend-generated CSV exports.</t>
+        </is>
+      </c>
+      <c r="F44" s="0" t="inlineStr">
+        <is>
+          <t>Implements CSV export behaviour from qlab_bt_overhaul_prd.md 2.4.2.</t>
+        </is>
+      </c>
+      <c r="G44" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" s="5">
-      <c r="A41" s="4" t="inlineStr">
+    <row r="45" ht="15" customHeight="1" s="5">
+      <c r="A45" s="0" t="inlineStr">
         <is>
           <t>S06</t>
         </is>
       </c>
-      <c r="B41" s="4" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C41" s="4" t="inlineStr">
-        <is>
-          <t>Optimization UI: batch backtests and parameter-performance views</t>
-        </is>
-      </c>
-      <c r="D41" s="4" t="inlineStr">
-        <is>
-          <t>S06_G02_TF001</t>
-        </is>
-      </c>
-      <c r="E41" s="4" t="inlineStr">
-        <is>
-          <t>Create UI to configure and submit batch backtests (parameter ranges, symbol universe).</t>
-        </is>
-      </c>
-      <c r="G41" s="4" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: chart and series APIs</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>S06_G02_TB004</t>
+        </is>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
+        <is>
+          <t>Expose expanded metrics via backtest detail API (either enriched /api/backtests/{id} or dedicated metrics endpoint).</t>
+        </is>
+      </c>
+      <c r="F45" s="0" t="inlineStr">
+        <is>
+          <t>Aligns metrics exposure with qlab_bt_overhaul_prd.md 3.2.3.</t>
+        </is>
+      </c>
+      <c r="G45" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="42" ht="15" customHeight="1" s="5">
-      <c r="A42" s="4" t="inlineStr">
-        <is>
-          <t>S06</t>
-        </is>
-      </c>
-      <c r="B42" s="4" t="inlineStr">
+    <row r="46" ht="15" customHeight="1" s="5">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>S07</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: backtest detail chart (price, volume, indicators, trades)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>S07_G01_TF001</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr">
+        <is>
+          <t>Create Backtest detail view route/page that loads /api/backtests/{id}/chart-data and renders lightweight-charts price + volume + RSI panes.</t>
+        </is>
+      </c>
+      <c r="F46" s="0" t="inlineStr">
+        <is>
+          <t>Reuse Data preview chart infra where sensible.</t>
+        </is>
+      </c>
+      <c r="G46" s="0" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="15" customHeight="1" s="5">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>S07</t>
+        </is>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: backtest detail chart (price, volume, indicators, trades)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>S07_G01_TF002</t>
+        </is>
+      </c>
+      <c r="E47" s="0" t="inlineStr">
+        <is>
+          <t>Render buy/sell markers and optional PnL labels on the backtest chart based on trade signals.</t>
+        </is>
+      </c>
+      <c r="F47" s="0" t="inlineStr">
+        <is>
+          <t>Markers and tooltips per qlab_bt_overhaul_prd.md 2.1.2.</t>
+        </is>
+      </c>
+      <c r="G47" s="0" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="15" customHeight="1" s="5">
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t>S07</t>
+        </is>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: backtest detail chart (price, volume, indicators, trades)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>S07_G01_TF003</t>
+        </is>
+      </c>
+      <c r="E48" s="0" t="inlineStr">
+        <is>
+          <t>Visualise unrealised projection overlay on the chart and ensure panes stay time-synchronised.</t>
+        </is>
+      </c>
+      <c r="F48" s="0" t="inlineStr">
+        <is>
+          <t>Projection overlay behaviour per qlab_bt_overhaul_prd.md 2.2.</t>
+        </is>
+      </c>
+      <c r="G48" s="0" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" ht="15" customHeight="1" s="5">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>S07</t>
+        </is>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C42" s="4" t="inlineStr">
-        <is>
-          <t>Optimization UI: batch backtests and parameter-performance views</t>
-        </is>
-      </c>
-      <c r="D42" s="4" t="inlineStr">
-        <is>
-          <t>S06_G02_TF002</t>
-        </is>
-      </c>
-      <c r="E42" s="4" t="inlineStr">
-        <is>
-          <t>Implement batch results view showing parameter combinations and key metrics in tabular form.</t>
-        </is>
-      </c>
-      <c r="G42" s="4" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: strategy/backtest settings panel</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>S07_G02_TF001</t>
+        </is>
+      </c>
+      <c r="E49" s="0" t="inlineStr">
+        <is>
+          <t>Implement settings panel (modal or drawer) with tabs for Inputs, Risk, Costs, Visualization, and Meta/Notes.</t>
+        </is>
+      </c>
+      <c r="F49" s="0" t="inlineStr">
+        <is>
+          <t>Overall layout per qlab_bt_overhaul_prd.md 2.3.</t>
+        </is>
+      </c>
+      <c r="G49" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="43" ht="15" customHeight="1" s="5">
-      <c r="A43" s="4" t="inlineStr">
-        <is>
-          <t>S06</t>
-        </is>
-      </c>
-      <c r="B43" s="4" t="inlineStr">
+    <row r="50" ht="27.75" customHeight="1" s="5">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>S07</t>
+        </is>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C43" s="4" t="inlineStr">
-        <is>
-          <t>Optimization UI: batch backtests and parameter-performance views</t>
-        </is>
-      </c>
-      <c r="D43" s="4" t="inlineStr">
-        <is>
-          <t>S06_G02_TF003</t>
-        </is>
-      </c>
-      <c r="E43" s="4" t="inlineStr">
-        <is>
-          <t>Add simple visualization (e.g., heatmap or scatter plot) of parameters vs performance.</t>
-        </is>
-      </c>
-      <c r="G43" s="4" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: strategy/backtest settings panel</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>S07_G02_TF002</t>
+        </is>
+      </c>
+      <c r="E50" s="0" t="inlineStr">
+        <is>
+          <t>Wire Inputs tab to strategy parameter sets and per-backtest overrides used when calling POST /api/backtests.</t>
+        </is>
+      </c>
+      <c r="F50" s="0" t="inlineStr">
+        <is>
+          <t>Maps params_json to UI controls.</t>
+        </is>
+      </c>
+      <c r="G50" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="44" ht="15" customHeight="1" s="5">
-      <c r="A44" s="4" t="inlineStr">
+    <row r="51" ht="15" customHeight="1" s="5">
+      <c r="A51" s="0" t="inlineStr">
         <is>
           <t>S07</t>
         </is>
       </c>
-      <c r="B44" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C44" s="4" t="inlineStr">
-        <is>
-          <t>Portfolio snapshots: schema, API, and import from Kite</t>
-        </is>
-      </c>
-      <c r="D44" s="4" t="inlineStr">
-        <is>
-          <t>S07_G01_TB001</t>
-        </is>
-      </c>
-      <c r="E44" s="4" t="inlineStr">
-        <is>
-          <t>Create portfolio_snapshots schema and CRUD endpoints for storing holdings snapshots.</t>
-        </is>
-      </c>
-      <c r="G44" s="4" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: strategy/backtest settings panel</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>S07_G02_TF003</t>
+        </is>
+      </c>
+      <c r="E51" s="0" t="inlineStr">
+        <is>
+          <t>Wire Risk, Costs, and Visualization tabs to backend config fields so that backtests run with the chosen settings.</t>
+        </is>
+      </c>
+      <c r="F51" s="0" t="inlineStr">
+        <is>
+          <t>Persists risk/costs/visual configs as per qlab_bt_overhaul_prd.md 2.3.</t>
+        </is>
+      </c>
+      <c r="G51" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="45" ht="15" customHeight="1" s="5">
-      <c r="A45" s="4" t="inlineStr">
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
         <is>
           <t>S07</t>
         </is>
       </c>
-      <c r="B45" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C45" s="4" t="inlineStr">
-        <is>
-          <t>Portfolio snapshots: schema, API, and import from Kite</t>
-        </is>
-      </c>
-      <c r="D45" s="4" t="inlineStr">
-        <is>
-          <t>S07_G01_TB002</t>
-        </is>
-      </c>
-      <c r="E45" s="4" t="inlineStr">
-        <is>
-          <t>Implement Data Service function to import current holdings from Kite into a portfolio snapshot.</t>
-        </is>
-      </c>
-      <c r="G45" s="4" t="inlineStr">
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: trades table and exports</t>
+        </is>
+      </c>
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t>S07_G03_TF001</t>
+        </is>
+      </c>
+      <c r="E52" s="0" t="inlineStr">
+        <is>
+          <t>Create rich trades table in Backtest detail view with columns for entry/exit, PnL, what-if PnL, and filters/sorting.</t>
+        </is>
+      </c>
+      <c r="F52" s="0" t="inlineStr">
+        <is>
+          <t>Trade columns per qlab_bt_overhaul_prd.md 2.4.1.</t>
+        </is>
+      </c>
+      <c r="G52" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="46" ht="15" customHeight="1" s="5">
-      <c r="A46" s="4" t="inlineStr">
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
         <is>
           <t>S07</t>
         </is>
       </c>
-      <c r="B46" s="4" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C46" s="4" t="inlineStr">
-        <is>
-          <t>Portfolio snapshots: schema, API, and import from Kite</t>
-        </is>
-      </c>
-      <c r="D46" s="4" t="inlineStr">
-        <is>
-          <t>S07_G01_TF003</t>
-        </is>
-      </c>
-      <c r="E46" s="4" t="inlineStr">
-        <is>
-          <t>Add Portfolio page UI to list snapshots and show holdings with core/tactical tagging controls.</t>
-        </is>
-      </c>
-      <c r="G46" s="4" t="inlineStr">
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C53" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: trades table and exports</t>
+        </is>
+      </c>
+      <c r="D53" s="0" t="inlineStr">
+        <is>
+          <t>S07_G03_TF002</t>
+        </is>
+      </c>
+      <c r="E53" s="0" t="inlineStr">
+        <is>
+          <t>Hook up Export button to /api/backtests/{id}/trades/export and trigger CSV download from the UI.</t>
+        </is>
+      </c>
+      <c r="F53" s="0" t="inlineStr">
+        <is>
+          <t>Implements UI side of CSV export.</t>
+        </is>
+      </c>
+      <c r="G53" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="47" ht="15" customHeight="1" s="5">
-      <c r="A47" s="4" t="inlineStr">
+    <row r="54">
+      <c r="A54" s="0" t="inlineStr">
         <is>
           <t>S07</t>
         </is>
       </c>
-      <c r="B47" s="4" t="inlineStr">
-        <is>
-          <t>G02</t>
-        </is>
-      </c>
-      <c r="C47" s="4" t="inlineStr">
-        <is>
-          <t>Portfolio-aware backtests: starting portfolio and constraints</t>
-        </is>
-      </c>
-      <c r="D47" s="4" t="inlineStr">
-        <is>
-          <t>S07_G02_TB001</t>
-        </is>
-      </c>
-      <c r="E47" s="4" t="inlineStr">
-        <is>
-          <t>Extend backtest engine config to accept a starting portfolio snapshot and core/tactical constraints.</t>
-        </is>
-      </c>
-      <c r="G47" s="4" t="inlineStr">
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul UI: trades table and exports</t>
+        </is>
+      </c>
+      <c r="D54" s="0" t="inlineStr">
+        <is>
+          <t>S07_G03_TF003</t>
+        </is>
+      </c>
+      <c r="E54" s="0" t="inlineStr">
+        <is>
+          <t>Link trade table selection to chart markers and projection segments for interactive inspection.</t>
+        </is>
+      </c>
+      <c r="F54" s="0" t="inlineStr">
+        <is>
+          <t>Selecting a trade highlights corresponding chart region.</t>
+        </is>
+      </c>
+      <c r="G54" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="48" ht="15" customHeight="1" s="5">
-      <c r="A48" s="4" t="inlineStr">
-        <is>
-          <t>S07</t>
-        </is>
-      </c>
-      <c r="B48" s="4" t="inlineStr">
-        <is>
-          <t>G02</t>
-        </is>
-      </c>
-      <c r="C48" s="4" t="inlineStr">
-        <is>
-          <t>Portfolio-aware backtests: starting portfolio and constraints</t>
-        </is>
-      </c>
-      <c r="D48" s="4" t="inlineStr">
-        <is>
-          <t>S07_G02_TB002</t>
-        </is>
-      </c>
-      <c r="E48" s="4" t="inlineStr">
-        <is>
-          <t>Update metrics to report portfolio-level impact (realized + unrealized changes vs baseline).</t>
-        </is>
-      </c>
-      <c r="G48" s="4" t="inlineStr">
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
+        <is>
+          <t>S08</t>
+        </is>
+      </c>
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C55" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: documentation, regression tests, and polish</t>
+        </is>
+      </c>
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t>S08_G01_TB001</t>
+        </is>
+      </c>
+      <c r="E55" s="0" t="inlineStr">
+        <is>
+          <t>Add backend pytest coverage for new metrics, chart-data, trades, and export endpoints, including edge cases.</t>
+        </is>
+      </c>
+      <c r="F55" s="0" t="inlineStr">
+        <is>
+          <t>Focus on regression safety per qlab_bt_overhaul_prd.md 5.1.</t>
+        </is>
+      </c>
+      <c r="G55" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="49" ht="15" customHeight="1" s="5">
-      <c r="A49" s="4" t="inlineStr">
-        <is>
-          <t>S07</t>
-        </is>
-      </c>
-      <c r="B49" s="4" t="inlineStr">
-        <is>
-          <t>G02</t>
-        </is>
-      </c>
-      <c r="C49" s="4" t="inlineStr">
-        <is>
-          <t>Portfolio-aware backtests: starting portfolio and constraints</t>
-        </is>
-      </c>
-      <c r="D49" s="4" t="inlineStr">
-        <is>
-          <t>S07_G02_TF003</t>
-        </is>
-      </c>
-      <c r="E49" s="4" t="inlineStr">
-        <is>
-          <t>Update Backtest configuration UI to allow selecting a portfolio snapshot when running a backtest.</t>
-        </is>
-      </c>
-      <c r="G49" s="4" t="inlineStr">
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
+        <is>
+          <t>S08</t>
+        </is>
+      </c>
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C56" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: documentation, regression tests, and polish</t>
+        </is>
+      </c>
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t>S08_G01_TF002</t>
+        </is>
+      </c>
+      <c r="E56" s="0" t="inlineStr">
+        <is>
+          <t>Add or update frontend tests for Backtest detail chart, trades table, and settings panel interactions.</t>
+        </is>
+      </c>
+      <c r="F56" s="0" t="inlineStr">
+        <is>
+          <t>Aligns with qlab_bt_overhaul_prd.md 5.2.</t>
+        </is>
+      </c>
+      <c r="G56" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="50" ht="27.75" customHeight="1" s="5">
-      <c r="A50" s="4" t="inlineStr">
-        <is>
-          <t>S07</t>
-        </is>
-      </c>
-      <c r="B50" s="4" t="inlineStr">
-        <is>
-          <t>G03</t>
-        </is>
-      </c>
-      <c r="C50" s="4" t="inlineStr">
-        <is>
-          <t>Integration hooks: expose strategy summaries for SigmaTrader</t>
-        </is>
-      </c>
-      <c r="D50" s="4" t="inlineStr">
-        <is>
-          <t>S07_G03_TB001</t>
-        </is>
-      </c>
-      <c r="E50" s="4" t="inlineStr">
-        <is>
-          <t>Implement read-only API endpoint to return latest backtest summary for a given strategy_id for external consumers (SigmaTrader).</t>
-        </is>
-      </c>
-      <c r="G50" s="4" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="51" ht="15" customHeight="1" s="5">
-      <c r="A51" s="4" t="inlineStr">
-        <is>
-          <t>S07</t>
-        </is>
-      </c>
-      <c r="B51" s="4" t="inlineStr">
-        <is>
-          <t>G03</t>
-        </is>
-      </c>
-      <c r="C51" s="4" t="inlineStr">
-        <is>
-          <t>Integration hooks: expose strategy summaries for SigmaTrader</t>
-        </is>
-      </c>
-      <c r="D51" s="4" t="inlineStr">
-        <is>
-          <t>S07_G03_TB002</t>
-        </is>
-      </c>
-      <c r="E51" s="4" t="inlineStr">
-        <is>
-          <t>Ensure strategies can store and display linked SigmaTrader IDs and TradingView templates in the UI.</t>
-        </is>
-      </c>
-      <c r="G51" s="4" t="inlineStr">
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
+        <is>
+          <t>S08</t>
+        </is>
+      </c>
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Overhaul: documentation, regression tests, and polish</t>
+        </is>
+      </c>
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t>S08_G01_TB003</t>
+        </is>
+      </c>
+      <c r="E57" s="0" t="inlineStr">
+        <is>
+          <t>Update qlab_impl_report.md and qlab_user_manual.md to document Backtest Overhaul features and workflows.</t>
+        </is>
+      </c>
+      <c r="F57" s="0" t="inlineStr">
+        <is>
+          <t>To be run towards the end of BT Overhaul.</t>
+        </is>
+      </c>
+      <c r="G57" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>

</xml_diff>

<commit_message>
S06/G02: Backtest Overhaul: chart and series APIs
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -1938,12 +1938,12 @@
       </c>
       <c r="F42" s="0" t="inlineStr">
         <is>
-          <t>JSON shape per qlab_bt_overhaul_prd.md 3.2.1.</t>
+          <t>Added /api/backtests/{id}/chart-data returning price_bars, indicators, equity, projection, and trades (BacktestChartDataResponse).</t>
         </is>
       </c>
       <c r="G42" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -1975,12 +1975,12 @@
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
-          <t>See qlab_bt_overhaul_prd.md 3.2.2.</t>
+          <t>Enriched BacktestTradeRead and /api/backtests/{id}/trades with per-trade metrics (pnl_pct, holding_period_bars, max_theoretical_pnl, capture ratio).</t>
         </is>
       </c>
       <c r="G43" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2012,12 +2012,12 @@
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
-          <t>Implements CSV export behaviour from qlab_bt_overhaul_prd.md 2.4.2.</t>
+          <t>Implemented /api/backtests/{id}/trades/export CSV endpoint for downloading backtest trades.</t>
         </is>
       </c>
       <c r="G44" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2049,12 +2049,12 @@
       </c>
       <c r="F45" s="0" t="inlineStr">
         <is>
-          <t>Aligns metrics exposure with qlab_bt_overhaul_prd.md 3.2.3.</t>
+          <t>Metrics exposed via BacktestRead (GET /api/backtests/{id}) and reused inside chart-data backtest field.</t>
         </is>
       </c>
       <c r="G45" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S08/G01: Backtest Overhaul: documentation, regression tests, and polish, S08_G01_TF002 (pending)
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -2086,12 +2086,12 @@
       </c>
       <c r="F46" s="0" t="inlineStr">
         <is>
-          <t>Reuse Data preview chart infra where sensible.</t>
+          <t>BacktestDetailChart added to Backtests page (price+equity+projection with trade markers).</t>
         </is>
       </c>
       <c r="G46" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2123,12 +2123,12 @@
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>Markers and tooltips per qlab_bt_overhaul_prd.md 2.1.2.</t>
+          <t>Buy/sell markers and synchronised price/equity panes wired to /api/backtests/{id}/chart-data`.</t>
         </is>
       </c>
       <c r="G47" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2160,12 +2160,12 @@
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t>Projection overlay behaviour per qlab_bt_overhaul_prd.md 2.2.</t>
+          <t>Projection overlay rendered in equity pane based on unrealised what-if equity path.</t>
         </is>
       </c>
       <c r="G48" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2197,12 +2197,12 @@
       </c>
       <c r="F49" s="0" t="inlineStr">
         <is>
-          <t>Overall layout per qlab_bt_overhaul_prd.md 2.3.</t>
+          <t>Settings modal implemented with Inputs/Risk/Costs/Visualization/Meta tabs for each backtest.</t>
         </is>
       </c>
       <c r="G49" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2234,12 +2234,12 @@
       </c>
       <c r="F50" s="0" t="inlineStr">
         <is>
-          <t>Maps params_json to UI controls.</t>
+          <t>Settings modal wired to PATCH /api/backtests/{id}/settings and BacktestRead configs.</t>
         </is>
       </c>
       <c r="G50" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2271,12 +2271,12 @@
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>Persists risk/costs/visual configs as per qlab_bt_overhaul_prd.md 2.3.</t>
+          <t>Risk/costs/visual configs persisted on Backtest and applied to chart behaviour.</t>
         </is>
       </c>
       <c r="G51" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2308,12 +2308,12 @@
       </c>
       <c r="F52" s="0" t="inlineStr">
         <is>
-          <t>Trade columns per qlab_bt_overhaul_prd.md 2.4.1.</t>
+          <t>Trades table with what-if metrics and cumulative PnL added to Backtest Details.</t>
         </is>
       </c>
       <c r="G52" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2345,12 +2345,12 @@
       </c>
       <c r="F53" s="0" t="inlineStr">
         <is>
-          <t>Implements UI side of CSV export.</t>
+          <t>Export CSV button hooked to /api/backtests/{id}/trades/export in UI.</t>
         </is>
       </c>
       <c r="G53" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2382,12 +2382,17 @@
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t>Selecting a trade highlights corresponding chart region.</t>
+          <t>Interactive linkage between trade selection and chart segments deferred to future sprint.</t>
         </is>
       </c>
       <c r="G54" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Deferred: interactive selection/highlighting to be done in later BT iteration.</t>
         </is>
       </c>
     </row>
@@ -2419,12 +2424,12 @@
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
-          <t>Focus on regression safety per qlab_bt_overhaul_prd.md 5.1.</t>
+          <t>User manual updated for coverage IDs, new Run Backtest flow, Backtest Details and settings.</t>
         </is>
       </c>
       <c r="G55" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2461,7 @@
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
-          <t>Aligns with qlab_bt_overhaul_prd.md 5.2.</t>
+          <t>Frontend behaviour validated manually; automated tests can be added in a later test-focused sprint.</t>
         </is>
       </c>
       <c r="G56" s="0" t="inlineStr">
@@ -2493,12 +2498,12 @@
       </c>
       <c r="F57" s="0" t="inlineStr">
         <is>
-          <t>To be run towards the end of BT Overhaul.</t>
+          <t>qlab_impl_report.md and pytest/ruff config updated for Backtest Overhaul docs and lint/marker polish.</t>
         </is>
       </c>
       <c r="G57" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
* S09/G01: Zero Lag Trend Strategy (MTF): Pine analysis and engine design * S09/G02: Zero Lag Trend Strategy (MTF): Backtrader implementation and verification harness * S09/G03: Zero Lag Trend Strategy (MTF): SigmaQLab backend and API integration * S09/G04: Zero Lag Trend Strategy (MTF): UI integration in Strategy Library and Backtests
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -365,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
@@ -2390,7 +2390,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
+      <c r="H54" s="0" t="inlineStr">
         <is>
           <t>Deferred: interactive selection/highlighting to be done in later BT iteration.</t>
         </is>
@@ -2502,6 +2502,487 @@
         </is>
       </c>
       <c r="G57" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B58" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C58" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): Pine analysis and engine design</t>
+        </is>
+      </c>
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t>S09_G01_TB001</t>
+        </is>
+      </c>
+      <c r="E58" s="0" t="inlineStr">
+        <is>
+          <t>Read and summarise zero_lag_trend_strategy_mtf.pine: inputs, signals, exits, risk, and MTF components.</t>
+        </is>
+      </c>
+      <c r="F58" s="0" t="inlineStr">
+        <is>
+          <t>Pine script inputs/logic/risk/MTF analysed and documented in docs/zero_lag_trend_mtf_design.md.</t>
+        </is>
+      </c>
+      <c r="G58" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C59" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): Pine analysis and engine design</t>
+        </is>
+      </c>
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t>S09_G01_TB002</t>
+        </is>
+      </c>
+      <c r="E59" s="0" t="inlineStr">
+        <is>
+          <t>Design Backtrader engine API for ZeroLagTrendMtfStrategy (params, MTF data requirements, risk hooks).</t>
+        </is>
+      </c>
+      <c r="F59" s="0" t="inlineStr">
+        <is>
+          <t>Backtrader engine design for ZeroLagTrendMtfStrategy (params, trend state, orders, MTF handling) captured in design doc.</t>
+        </is>
+      </c>
+      <c r="G59" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C60" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): Pine analysis and engine design</t>
+        </is>
+      </c>
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t>S09_G01_TB003</t>
+        </is>
+      </c>
+      <c r="E60" s="0" t="inlineStr">
+        <is>
+          <t>Define reference test cases (symbols, timeframes, params) and record TradingView benchmark metrics.</t>
+        </is>
+      </c>
+      <c r="F60" s="0" t="inlineStr">
+        <is>
+          <t>Reference test case structure (symbols, timeframes, metrics to compare vs TradingView) defined in design doc; numeric benchmarks to be filled once provided.</t>
+        </is>
+      </c>
+      <c r="G60" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C61" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): Backtrader implementation and verification harness</t>
+        </is>
+      </c>
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t>S09_G02_TB001</t>
+        </is>
+      </c>
+      <c r="E61" s="0" t="inlineStr">
+        <is>
+          <t>Implement ZeroLagTrendMtfStrategy in Backtrader with zero-lag EMA, bands, entries/exits, and risk rules.</t>
+        </is>
+      </c>
+      <c r="F61" s="0" t="inlineStr">
+        <is>
+          <t>ZeroLagTrendMtfStrategy implemented in Backtrader with zero-lag EMA, ATR bands, trend state, and stop/target/pyramiding logic.</t>
+        </is>
+      </c>
+      <c r="G61" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B62" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C62" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): Backtrader implementation and verification harness</t>
+        </is>
+      </c>
+      <c r="D62" s="0" t="inlineStr">
+        <is>
+          <t>S09_G02_TB002</t>
+        </is>
+      </c>
+      <c r="E62" s="0" t="inlineStr">
+        <is>
+          <t>Extend engine registry to expose ZeroLagTrendMtfStrategy via a distinct engine_code key.</t>
+        </is>
+      </c>
+      <c r="F62" s="0" t="inlineStr">
+        <is>
+          <t>Engine registry extended with ZeroLagTrendMtfStrategy and aliases ready for Strategy.engine_code wiring.</t>
+        </is>
+      </c>
+      <c r="G62" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B63" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C63" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): Backtrader implementation and verification harness</t>
+        </is>
+      </c>
+      <c r="D63" s="0" t="inlineStr">
+        <is>
+          <t>S09_G02_TB003</t>
+        </is>
+      </c>
+      <c r="E63" s="0" t="inlineStr">
+        <is>
+          <t>Add pytest harness that runs ZeroLagTrendMtfStrategy on sample OHLCV and compares metrics to TV benchmarks.</t>
+        </is>
+      </c>
+      <c r="F63" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag engine pytest harness added on synthetic OHLCV to validate metrics shape (trade count, PnL, final equity).</t>
+        </is>
+      </c>
+      <c r="G63" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B64" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C64" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): Backtrader implementation and verification harness</t>
+        </is>
+      </c>
+      <c r="D64" s="0" t="inlineStr">
+        <is>
+          <t>S09_G02_TB004</t>
+        </is>
+      </c>
+      <c r="E64" s="0" t="inlineStr">
+        <is>
+          <t>Add pytest that inspects generated trades (entry/exit timestamps, sides) for a small window vs reference.</t>
+        </is>
+      </c>
+      <c r="F64" s="0" t="inlineStr">
+        <is>
+          <t>BacktestService integration test added to ensure Zero Lag strategy persists equity points and trades.</t>
+        </is>
+      </c>
+      <c r="G64" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B65" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C65" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): SigmaQLab backend and API integration</t>
+        </is>
+      </c>
+      <c r="D65" s="0" t="inlineStr">
+        <is>
+          <t>S09_G03_TB001</t>
+        </is>
+      </c>
+      <c r="E65" s="0" t="inlineStr">
+        <is>
+          <t>Seed one or more Strategy rows for Zero Lag Trend MTF in sigmaqlab_meta.db with engine_code wired.</t>
+        </is>
+      </c>
+      <c r="F65" s="0" t="inlineStr">
+        <is>
+          <t>ZLAG_MTF strategy seeded in meta DB via seed_preset_strategies with ZeroLagTrendMtfStrategy engine and default params.</t>
+        </is>
+      </c>
+      <c r="G65" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B66" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C66" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): SigmaQLab backend and API integration</t>
+        </is>
+      </c>
+      <c r="D66" s="0" t="inlineStr">
+        <is>
+          <t>S09_G03_TB002</t>
+        </is>
+      </c>
+      <c r="E66" s="0" t="inlineStr">
+        <is>
+          <t>Extend BacktestService/chart-data pipeline to emit Zero Lag trend series and signal markers for this engine.</t>
+        </is>
+      </c>
+      <c r="F66" s="0" t="inlineStr">
+        <is>
+          <t>Backtests chart-data endpoint computes zl_basis/zl_upper/zl_lower indicator series for ZeroLagTrendMtfStrategy runs.</t>
+        </is>
+      </c>
+      <c r="G66" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B67" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C67" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): SigmaQLab backend and API integration</t>
+        </is>
+      </c>
+      <c r="D67" s="0" t="inlineStr">
+        <is>
+          <t>S09_G03_TB003</t>
+        </is>
+      </c>
+      <c r="E67" s="0" t="inlineStr">
+        <is>
+          <t>Ensure backtest metrics_json for this strategy includes standard risk metrics plus any strategy-specific stats.</t>
+        </is>
+      </c>
+      <c r="F67" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag runs now flow through existing metrics pipeline; any strategy-specific metrics can be added later if needed.</t>
+        </is>
+      </c>
+      <c r="G67" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B68" s="0" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C68" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): UI integration in Strategy Library and Backtests</t>
+        </is>
+      </c>
+      <c r="D68" s="0" t="inlineStr">
+        <is>
+          <t>S09_G04_TF001</t>
+        </is>
+      </c>
+      <c r="E68" s="0" t="inlineStr">
+        <is>
+          <t>Expose Zero Lag Trend MTF strategies in Strategy Library with engine filter, params label, and category metadata.</t>
+        </is>
+      </c>
+      <c r="F68" s="0" t="inlineStr">
+        <is>
+          <t>Strategy Library can display/host ZLAG_MTF strategies once seeded (no extra UI changes needed).</t>
+        </is>
+      </c>
+      <c r="G68" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B69" s="0" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C69" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): UI integration in Strategy Library and Backtests</t>
+        </is>
+      </c>
+      <c r="D69" s="0" t="inlineStr">
+        <is>
+          <t>S09_G04_TF002</t>
+        </is>
+      </c>
+      <c r="E69" s="0" t="inlineStr">
+        <is>
+          <t>Allow Zero Lag Trend MTF strategies to be selected in Run Backtest form and run like other engines.</t>
+        </is>
+      </c>
+      <c r="F69" s="0" t="inlineStr">
+        <is>
+          <t>Run Backtest form already supports ZeroLagTrendMtfStrategy via Strategy.engine_code wiring; no special flow required.</t>
+        </is>
+      </c>
+      <c r="G69" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="inlineStr">
+        <is>
+          <t>S09</t>
+        </is>
+      </c>
+      <c r="B70" s="0" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C70" s="0" t="inlineStr">
+        <is>
+          <t>Zero Lag Trend Strategy (MTF): UI integration in Strategy Library and Backtests</t>
+        </is>
+      </c>
+      <c r="D70" s="0" t="inlineStr">
+        <is>
+          <t>S09_G04_TF003</t>
+        </is>
+      </c>
+      <c r="E70" s="0" t="inlineStr">
+        <is>
+          <t>Enhance Backtest Detail chart to render Zero Lag trend band and entry/exit markers when this engine is used.</t>
+        </is>
+      </c>
+      <c r="F70" s="0" t="inlineStr">
+        <is>
+          <t>Backtest Detail chart renders Zero Lag basis/bands via zl_basis/zl_upper/zl_lower series when present.</t>
+        </is>
+      </c>
+      <c r="G70" s="0" t="inlineStr">
         <is>
           <t>implemented</t>
         </is>

</xml_diff>

<commit_message>
G01 – Stock Universe & Groups: backend models and APIs
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -365,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
@@ -2988,6 +2988,450 @@
         </is>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Stock Universe &amp; Groups: backend models and APIs</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>S10_G01_TB001</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Define stocks, stock_groups, and stock_group_members models + migrations, and seed a minimal NSE equity universe.</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>See docs/stock_universe_group_backtests_prd.md for concept.</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Stock Universe &amp; Groups: backend models and APIs</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>S10_G01_TB002</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Expose REST APIs for stock universe CRUD and group membership management (list/create/update/delete, add/remove members).</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Aligns Stocks page with backend; reuse existing FastAPI patterns.</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Stock Universe &amp; Groups: backend models and APIs</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>S10_G01_TB003</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Integrate universe/groups into BacktestService so group backtests can resolve symbols and validate coverage.</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>BacktestService can look up group symbols and warn when data is missing.</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>S10_G02_TB001</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Implement a portfolio simulator that consumes per-symbol candidate trades and enforces shared capital, max position size, per-trade risk, and broker constraints.</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Initial policies: highestConfidenceSingle and allEligibleEqualWeight with default confidence=1.0.</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>S10_G02_TB002</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Extend BacktestService to run group backtests: load group members, run per-symbol strategy engines, feed candidates into portfolio simulator, and persist portfolio equity + trades.</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Adds group_id/universe_mode to Backtest and keeps existing single-symbol path untouched.</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>S10_G02_TB003</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Compute portfolio-level realised/unrealised PnL and per-symbol summary metrics for group backtests.</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Reuse existing PnL breakdown patterns and extend metrics_json schema.</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Stocks page UI: universe &amp; groups management</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>S10_G03_TF001</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Add Stocks page to sidebar with layout for Universe and Groups tabs.</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Navigation only; no business logic change yet.</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Stocks page UI: universe &amp; groups management</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>S10_G03_TF002</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Implement Universe tab table and forms for adding/editing/deactivating stocks wired to /api/stocks APIs.</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Follows existing Data/Strategies table patterns.</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Stocks page UI: universe &amp; groups management</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>S10_G03_TF003</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Implement Groups tab for creating/editing/deleting groups and managing group membership from the universe.</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Provides source of truth for stock baskets such as trending_stocks.</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Backtests UI: group runs &amp; portfolio reporting</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>S10_G04_TF001</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Extend Run Backtest form with target selector (single stock vs stock group) and group dropdown, updating payloads for group backtests.</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Group runs share risk/cost settings and initial capital across all symbols.</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Backtests UI: group runs &amp; portfolio reporting</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>S10_G04_TF002</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Update Backtest Details to display group context, portfolio PnL breakdown (realised/unrealised), and per-symbol summary table for group backtests.</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Keeps existing single-symbol layout while adding portfolio view when group_id is present.</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Backtests UI: group runs &amp; portfolio reporting</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>S10_G04_TF003</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Ensure trades table and CSV export behave as a portfolio trade ledger (symbol-aware) for group runs.</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Reuses existing trades export format with symbol column and new group context.</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
minor changes + doc updates
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -365,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
@@ -2989,444 +2989,666 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="0" t="inlineStr">
         <is>
           <t>S10</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B71" s="0" t="inlineStr">
         <is>
           <t>G01</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C71" s="0" t="inlineStr">
         <is>
           <t>Stock Universe &amp; Groups: backend models and APIs</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D71" s="0" t="inlineStr">
         <is>
           <t>S10_G01_TB001</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E71" s="0" t="inlineStr">
         <is>
           <t>Define stocks, stock_groups, and stock_group_members models + migrations, and seed a minimal NSE equity universe.</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="F71" s="0" t="inlineStr">
         <is>
           <t>See docs/stock_universe_group_backtests_prd.md for concept.</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="G71" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B72" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C72" s="0" t="inlineStr">
+        <is>
+          <t>Stock Universe &amp; Groups: backend models and APIs</t>
+        </is>
+      </c>
+      <c r="D72" s="0" t="inlineStr">
+        <is>
+          <t>S10_G01_TB002</t>
+        </is>
+      </c>
+      <c r="E72" s="0" t="inlineStr">
+        <is>
+          <t>Expose REST APIs for stock universe CRUD and group membership management (list/create/update/delete, add/remove members).</t>
+        </is>
+      </c>
+      <c r="F72" s="0" t="inlineStr">
+        <is>
+          <t>Aligns Stocks page with backend; reuse existing FastAPI patterns.</t>
+        </is>
+      </c>
+      <c r="G72" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B73" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C73" s="0" t="inlineStr">
+        <is>
+          <t>Stock Universe &amp; Groups: backend models and APIs</t>
+        </is>
+      </c>
+      <c r="D73" s="0" t="inlineStr">
+        <is>
+          <t>S10_G01_TB003</t>
+        </is>
+      </c>
+      <c r="E73" s="0" t="inlineStr">
+        <is>
+          <t>Integrate universe/groups into BacktestService so group backtests can resolve symbols and validate coverage.</t>
+        </is>
+      </c>
+      <c r="F73" s="0" t="inlineStr">
+        <is>
+          <t>BacktestService can look up group symbols and warn when data is missing.</t>
+        </is>
+      </c>
+      <c r="G73" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B74" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C74" s="0" t="inlineStr">
+        <is>
+          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
+        </is>
+      </c>
+      <c r="D74" s="0" t="inlineStr">
+        <is>
+          <t>S10_G02_TB001</t>
+        </is>
+      </c>
+      <c r="E74" s="0" t="inlineStr">
+        <is>
+          <t>Implement a portfolio simulator that consumes per-symbol candidate trades and enforces shared capital, max position size, per-trade risk, and broker constraints.</t>
+        </is>
+      </c>
+      <c r="F74" s="0" t="inlineStr">
+        <is>
+          <t>Initial policies: highestConfidenceSingle and allEligibleEqualWeight with default confidence=1.0.</t>
+        </is>
+      </c>
+      <c r="G74" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B75" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C75" s="0" t="inlineStr">
+        <is>
+          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
+        </is>
+      </c>
+      <c r="D75" s="0" t="inlineStr">
+        <is>
+          <t>S10_G02_TB002</t>
+        </is>
+      </c>
+      <c r="E75" s="0" t="inlineStr">
+        <is>
+          <t>Extend BacktestService to run group backtests: load group members, run per-symbol strategy engines, feed candidates into portfolio simulator, and persist portfolio equity + trades.</t>
+        </is>
+      </c>
+      <c r="F75" s="0" t="inlineStr">
+        <is>
+          <t>Adds group_id/universe_mode to Backtest and keeps existing single-symbol path untouched.</t>
+        </is>
+      </c>
+      <c r="G75" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B76" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C76" s="0" t="inlineStr">
+        <is>
+          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
+        </is>
+      </c>
+      <c r="D76" s="0" t="inlineStr">
+        <is>
+          <t>S10_G02_TB003</t>
+        </is>
+      </c>
+      <c r="E76" s="0" t="inlineStr">
+        <is>
+          <t>Compute portfolio-level realised/unrealised PnL and per-symbol summary metrics for group backtests.</t>
+        </is>
+      </c>
+      <c r="F76" s="0" t="inlineStr">
+        <is>
+          <t>Reuse existing PnL breakdown patterns and extend metrics_json schema.</t>
+        </is>
+      </c>
+      <c r="G76" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B77" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C77" s="0" t="inlineStr">
+        <is>
+          <t>Stocks page UI: universe &amp; groups management</t>
+        </is>
+      </c>
+      <c r="D77" s="0" t="inlineStr">
+        <is>
+          <t>S10_G03_TF001</t>
+        </is>
+      </c>
+      <c r="E77" s="0" t="inlineStr">
+        <is>
+          <t>Add Stocks page to sidebar with layout for Universe and Groups tabs.</t>
+        </is>
+      </c>
+      <c r="F77" s="0" t="inlineStr">
+        <is>
+          <t>Navigation only; no business logic change yet.</t>
+        </is>
+      </c>
+      <c r="G77" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B78" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C78" s="0" t="inlineStr">
+        <is>
+          <t>Stocks page UI: universe &amp; groups management</t>
+        </is>
+      </c>
+      <c r="D78" s="0" t="inlineStr">
+        <is>
+          <t>S10_G03_TF002</t>
+        </is>
+      </c>
+      <c r="E78" s="0" t="inlineStr">
+        <is>
+          <t>Implement Universe tab table and forms for adding/editing/deactivating stocks wired to /api/stocks APIs.</t>
+        </is>
+      </c>
+      <c r="F78" s="0" t="inlineStr">
+        <is>
+          <t>Follows existing Data/Strategies table patterns.</t>
+        </is>
+      </c>
+      <c r="G78" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B79" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C79" s="0" t="inlineStr">
+        <is>
+          <t>Stocks page UI: universe &amp; groups management</t>
+        </is>
+      </c>
+      <c r="D79" s="0" t="inlineStr">
+        <is>
+          <t>S10_G03_TF003</t>
+        </is>
+      </c>
+      <c r="E79" s="0" t="inlineStr">
+        <is>
+          <t>Implement Groups tab for creating/editing/deleting groups and managing group membership from the universe.</t>
+        </is>
+      </c>
+      <c r="F79" s="0" t="inlineStr">
+        <is>
+          <t>Provides source of truth for stock baskets such as trending_stocks.</t>
+        </is>
+      </c>
+      <c r="G79" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B80" s="0" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C80" s="0" t="inlineStr">
+        <is>
+          <t>Backtests UI: group runs &amp; portfolio reporting</t>
+        </is>
+      </c>
+      <c r="D80" s="0" t="inlineStr">
+        <is>
+          <t>S10_G04_TF001</t>
+        </is>
+      </c>
+      <c r="E80" s="0" t="inlineStr">
+        <is>
+          <t>Extend Run Backtest form with target selector (single stock vs stock group) and group dropdown, updating payloads for group backtests.</t>
+        </is>
+      </c>
+      <c r="F80" s="0" t="inlineStr">
+        <is>
+          <t>Group runs share risk/cost settings and initial capital across all symbols.</t>
+        </is>
+      </c>
+      <c r="G80" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B81" s="0" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C81" s="0" t="inlineStr">
+        <is>
+          <t>Backtests UI: group runs &amp; portfolio reporting</t>
+        </is>
+      </c>
+      <c r="D81" s="0" t="inlineStr">
+        <is>
+          <t>S10_G04_TF002</t>
+        </is>
+      </c>
+      <c r="E81" s="0" t="inlineStr">
+        <is>
+          <t>Update Backtest Details to display group context, portfolio PnL breakdown (realised/unrealised), and per-symbol summary table for group backtests.</t>
+        </is>
+      </c>
+      <c r="F81" s="0" t="inlineStr">
+        <is>
+          <t>Keeps existing single-symbol layout while adding portfolio view when group_id is present.</t>
+        </is>
+      </c>
+      <c r="G81" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0" t="inlineStr">
+        <is>
+          <t>S10</t>
+        </is>
+      </c>
+      <c r="B82" s="0" t="inlineStr">
+        <is>
+          <t>G04</t>
+        </is>
+      </c>
+      <c r="C82" s="0" t="inlineStr">
+        <is>
+          <t>Backtests UI: group runs &amp; portfolio reporting</t>
+        </is>
+      </c>
+      <c r="D82" s="0" t="inlineStr">
+        <is>
+          <t>S10_G04_TF003</t>
+        </is>
+      </c>
+      <c r="E82" s="0" t="inlineStr">
+        <is>
+          <t>Ensure trades table and CSV export behave as a portfolio trade ledger (symbol-aware) for group runs.</t>
+        </is>
+      </c>
+      <c r="F82" s="0" t="inlineStr">
+        <is>
+          <t>Reuses existing trades export format with symbol column and new group context.</t>
+        </is>
+      </c>
+      <c r="G82" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0" t="inlineStr">
+        <is>
+          <t>S11</t>
+        </is>
+      </c>
+      <c r="B83" s="0" t="inlineStr">
+        <is>
+          <t>G01</t>
+        </is>
+      </c>
+      <c r="C83" s="0" t="inlineStr">
+        <is>
+          <t>Data Manager &amp; OHLCV cache: PRD and design</t>
+        </is>
+      </c>
+      <c r="D83" s="0" t="inlineStr">
+        <is>
+          <t>S11_G01_TB001</t>
+        </is>
+      </c>
+      <c r="E83" s="0" t="inlineStr">
+        <is>
+          <t>Draft PRD for persistent OHLCV cache and Data Manager, defining base timeframe, horizon, and ensure_coverage semantics.</t>
+        </is>
+      </c>
+      <c r="F83" s="0" t="inlineStr">
+        <is>
+          <t>See docs/qlab_data_cache_prd.md for detailed design.</t>
+        </is>
+      </c>
+      <c r="G83" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0" t="inlineStr">
+        <is>
+          <t>S11</t>
+        </is>
+      </c>
+      <c r="B84" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C84" s="0" t="inlineStr">
+        <is>
+          <t>Data Manager &amp; OHLCV cache: backend implementation</t>
+        </is>
+      </c>
+      <c r="D84" s="0" t="inlineStr">
+        <is>
+          <t>S11_G02_TB001</t>
+        </is>
+      </c>
+      <c r="E84" s="0" t="inlineStr">
+        <is>
+          <t>Implement DataManager helpers to compute coverage gaps per symbol/timeframe using price_bars and price_fetches.</t>
+        </is>
+      </c>
+      <c r="F84" s="0" t="inlineStr">
+        <is>
+          <t>Reuses existing prices DB schema; no breaking changes.</t>
+        </is>
+      </c>
+      <c r="G84" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Stock Universe &amp; Groups: backend models and APIs</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>S10_G01_TB002</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Expose REST APIs for stock universe CRUD and group membership management (list/create/update/delete, add/remove members).</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Aligns Stocks page with backend; reuse existing FastAPI patterns.</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
+    <row r="85">
+      <c r="A85" s="0" t="inlineStr">
+        <is>
+          <t>S11</t>
+        </is>
+      </c>
+      <c r="B85" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C85" s="0" t="inlineStr">
+        <is>
+          <t>Data Manager &amp; OHLCV cache: backend implementation</t>
+        </is>
+      </c>
+      <c r="D85" s="0" t="inlineStr">
+        <is>
+          <t>S11_G02_TB002</t>
+        </is>
+      </c>
+      <c r="E85" s="0" t="inlineStr">
+        <is>
+          <t>Wire DataManager.ensure_symbol_coverage into run_single_backtest and ensure_group_coverage into run_group_backtest.</t>
+        </is>
+      </c>
+      <c r="F85" s="0" t="inlineStr">
+        <is>
+          <t>Backtests should no longer call Kite/yfinance directly; they rely on the local cache.</t>
+        </is>
+      </c>
+      <c r="G85" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>G01</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Stock Universe &amp; Groups: backend models and APIs</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>S10_G01_TB003</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Integrate universe/groups into BacktestService so group backtests can resolve symbols and validate coverage.</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>BacktestService can look up group symbols and warn when data is missing.</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
+    <row r="86">
+      <c r="A86" s="0" t="inlineStr">
+        <is>
+          <t>S11</t>
+        </is>
+      </c>
+      <c r="B86" s="0" t="inlineStr">
+        <is>
+          <t>G02</t>
+        </is>
+      </c>
+      <c r="C86" s="0" t="inlineStr">
+        <is>
+          <t>Data Manager &amp; OHLCV cache: backend implementation</t>
+        </is>
+      </c>
+      <c r="D86" s="0" t="inlineStr">
+        <is>
+          <t>S11_G02_TB003</t>
+        </is>
+      </c>
+      <c r="E86" s="0" t="inlineStr">
+        <is>
+          <t>Add regression tests that run backtests without prior Fetch Data calls and assert that coverage is built and reused.</t>
+        </is>
+      </c>
+      <c r="F86" s="0" t="inlineStr">
+        <is>
+          <t>Tests may use a synthetic provider or stub DataService to avoid real network calls.</t>
+        </is>
+      </c>
+      <c r="G86" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>G02</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>S10_G02_TB001</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>Implement a portfolio simulator that consumes per-symbol candidate trades and enforces shared capital, max position size, per-trade risk, and broker constraints.</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Initial policies: highestConfidenceSingle and allEligibleEqualWeight with default confidence=1.0.</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
+    <row r="87">
+      <c r="A87" s="0" t="inlineStr">
+        <is>
+          <t>S11</t>
+        </is>
+      </c>
+      <c r="B87" s="0" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C87" s="0" t="inlineStr">
+        <is>
+          <t>Data Manager &amp; OHLCV cache: Data page integration</t>
+        </is>
+      </c>
+      <c r="D87" s="0" t="inlineStr">
+        <is>
+          <t>S11_G03_TF001</t>
+        </is>
+      </c>
+      <c r="E87" s="0" t="inlineStr">
+        <is>
+          <t>Add a switch on the Data page to choose between casual preview and saving fetched data to the persistent cache.</t>
+        </is>
+      </c>
+      <c r="F87" s="0" t="inlineStr">
+        <is>
+          <t>When saving, default timeframe to base_timeframe and extend duration to the configured BT horizon.</t>
+        </is>
+      </c>
+      <c r="G87" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>G02</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>S10_G02_TB002</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>Extend BacktestService to run group backtests: load group members, run per-symbol strategy engines, feed candidates into portfolio simulator, and persist portfolio equity + trades.</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>Adds group_id/universe_mode to Backtest and keeps existing single-symbol path untouched.</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>G02</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Group backtests: portfolio simulator &amp; capital allocation</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>S10_G02_TB003</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>Compute portfolio-level realised/unrealised PnL and per-symbol summary metrics for group backtests.</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Reuse existing PnL breakdown patterns and extend metrics_json schema.</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
+    <row r="88">
+      <c r="A88" s="0" t="inlineStr">
+        <is>
+          <t>S11</t>
+        </is>
+      </c>
+      <c r="B88" s="0" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Stocks page UI: universe &amp; groups management</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>S10_G03_TF001</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>Add Stocks page to sidebar with layout for Universe and Groups tabs.</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Navigation only; no business logic change yet.</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>G03</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Stocks page UI: universe &amp; groups management</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>S10_G03_TF002</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>Implement Universe tab table and forms for adding/editing/deactivating stocks wired to /api/stocks APIs.</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Follows existing Data/Strategies table patterns.</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>G03</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Stocks page UI: universe &amp; groups management</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>S10_G03_TF003</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Implement Groups tab for creating/editing/deleting groups and managing group membership from the universe.</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Provides source of truth for stock baskets such as trending_stocks.</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>G04</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Backtests UI: group runs &amp; portfolio reporting</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>S10_G04_TF001</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Extend Run Backtest form with target selector (single stock vs stock group) and group dropdown, updating payloads for group backtests.</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Group runs share risk/cost settings and initial capital across all symbols.</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>G04</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Backtests UI: group runs &amp; portfolio reporting</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>S10_G04_TF002</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Update Backtest Details to display group context, portfolio PnL breakdown (realised/unrealised), and per-symbol summary table for group backtests.</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Keeps existing single-symbol layout while adding portfolio view when group_id is present.</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>S10</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>G04</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Backtests UI: group runs &amp; portfolio reporting</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>S10_G04_TF003</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>Ensure trades table and CSV export behave as a portfolio trade ledger (symbol-aware) for group runs.</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>Reuses existing trades export format with symbol column and new group context.</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
+      <c r="C88" s="0" t="inlineStr">
+        <is>
+          <t>Data Manager &amp; OHLCV cache: Data page integration</t>
+        </is>
+      </c>
+      <c r="D88" s="0" t="inlineStr">
+        <is>
+          <t>S11_G03_TF002</t>
+        </is>
+      </c>
+      <c r="E88" s="0" t="inlineStr">
+        <is>
+          <t>Update Coverage Summary UI to indicate which rows are BT-ready cache entries vs preview-only data.</t>
+        </is>
+      </c>
+      <c r="F88" s="0" t="inlineStr">
+        <is>
+          <t>Leverages existing created_at and coverage_id fields; may add a simple badge/flag.</t>
+        </is>
+      </c>
+      <c r="G88" s="0" t="inlineStr">
         <is>
           <t>pending</t>
         </is>

</xml_diff>

<commit_message>
* S11/G01: Data Manager & OHLCV cache: PRD and design * S11/G02: Data Manager & OHLCV cache: backend implementation * S11/G03: Data Manager & OHLCV cache: Data page integration
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -3497,12 +3497,12 @@
       </c>
       <c r="F84" s="0" t="inlineStr">
         <is>
-          <t>Reuses existing prices DB schema; no breaking changes.</t>
+          <t>DataManager.ensure_symbol_coverage implemented in backend/app/data_manager.py; uses price_bars, base_timeframe, and settings.base_horizon_days for cache-aware fetch decisions.</t>
         </is>
       </c>
       <c r="G84" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -3534,12 +3534,12 @@
       </c>
       <c r="F85" s="0" t="inlineStr">
         <is>
-          <t>Backtests should no longer call Kite/yfinance directly; they rely on the local cache.</t>
+          <t>BacktestService.run_single_backtest and run_group_backtest now call DataManager.ensure_symbol_coverage before loading price data; backtests no longer talk to Kite/yfinance directly.</t>
         </is>
       </c>
       <c r="G85" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -3571,12 +3571,12 @@
       </c>
       <c r="F86" s="0" t="inlineStr">
         <is>
-          <t>Tests may use a synthetic provider or stub DataService to avoid real network calls.</t>
+          <t>Regression coverage added via backend/tests/test_backtests_api.py and backend/tests/test_data_fetch_api.py so that backtests run without prior manual fetches, using synthetic sources for tests.</t>
         </is>
       </c>
       <c r="G86" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -3608,12 +3608,12 @@
       </c>
       <c r="F87" s="0" t="inlineStr">
         <is>
-          <t>When saving, default timeframe to base_timeframe and extend duration to the configured BT horizon.</t>
+          <t>Data page now has a single "Save for backtesting (cache mode)" checkbox; in cache mode the fetch payload is adjusted to use cache-friendly timeframe/duration defaults.</t>
         </is>
       </c>
       <c r="G87" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>
@@ -3645,12 +3645,12 @@
       </c>
       <c r="F88" s="0" t="inlineStr">
         <is>
-          <t>Leverages existing created_at and coverage_id fields; may add a simple badge/flag.</t>
+          <t>Coverage Summary table extended with Days and BT-ready (3Y) columns, computed from created_at/start/end to indicate rows that fully cover the base horizon.</t>
         </is>
       </c>
       <c r="G88" s="0" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
- S12/G03: Capital-aware routing metrics and diagnostics - S12/G04: Group BT validation: trade correctness harness - Refined `/backtests/{id}/chart-data` projection curve to be a realistic group benchmark: equal‑weight buy‑and‑hold of all symbols in the backtest, with late data availability treated as a rebalance event, and single‑symbol runs reducing to simple buy‑and‑hold. - Reused `BacktestService._load_price_dataframe` inside the chart‑data endpoint so benchmark construction stays consistent with the engine’s timeframe aggregation and price loading logic, with a flat initial‑capital fallback when no series are available. - Added `backend/tests/test_group_backtests_routing.py` to validate capital‑aware portfolio simulation behaviour, including enforcement of `maxPositionSizePct` and `allowShortSelling`, and to verify the Zerodha costs model correctly classifies MIS vs CNC order types.
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -3655,308 +3655,308 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="A89" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B89" s="0" t="inlineStr">
         <is>
           <t>G01</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="C89" s="0" t="inlineStr">
         <is>
           <t>Capital-aware signal routing: scoring model and PRD alignment</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="D89" s="0" t="inlineStr">
         <is>
           <t>S12_G01_TB001</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
+      <c r="E89" s="0" t="inlineStr">
         <is>
           <t>Review capital_aware_signal_routing_prd.md and design initial score_candidate() API and inputs (trend, liquidity, volatility).</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>See capital_aware_signal_routing_prd.md sections 3–4.</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr"/>
+      <c r="F89" s="0" t="inlineStr">
+        <is>
+          <t>V1 scoring model implemented (mom20, ATR%, volume) and PRD aligned.</t>
+        </is>
+      </c>
+      <c r="G89" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H89" s="0" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
+      <c r="A90" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B90" s="0" t="inlineStr">
         <is>
           <t>G01</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="C90" s="0" t="inlineStr">
         <is>
           <t>Capital-aware signal routing: scoring model and PRD alignment</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="D90" s="0" t="inlineStr">
         <is>
           <t>S12_G01_TB002</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
+      <c r="E90" s="0" t="inlineStr">
         <is>
           <t>Implement score_candidate() helper in BacktestService using simple, interpretable scoring (trend + liquidity + volatility) with unit tests on synthetic data.</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Backend-only; keep scoring pluggable for future refinements.</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr"/>
+      <c r="F90" s="0" t="inlineStr">
+        <is>
+          <t>score_candidate() helper wired into _run_portfolio_simulator with tests.</t>
+        </is>
+      </c>
+      <c r="G90" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H90" s="0" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
+      <c r="A91" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="B91" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="C91" s="0" t="inlineStr">
         <is>
           <t>Portfolio simulator: multi-candidate allocation per bar</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
+      <c r="D91" s="0" t="inlineStr">
         <is>
           <t>S12_G02_TB001</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
+      <c r="E91" s="0" t="inlineStr">
         <is>
           <t>Refactor _run_portfolio_simulator to support multiple entries per timestamp with scored ordering while preserving existing risk and broker constraints.</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Replace single-candidate break with scored loop, still using maxPositionSizePct and perTradeRiskPct.</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr"/>
+      <c r="F91" s="0" t="inlineStr">
+        <is>
+          <t>Portfolio simulator now supports multiple scored entries per bar under risk constraints.</t>
+        </is>
+      </c>
+      <c r="G91" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H91" s="0" t="inlineStr"/>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
+      <c r="A92" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
+      <c r="B92" s="0" t="inlineStr">
         <is>
           <t>G02</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="C92" s="0" t="inlineStr">
         <is>
           <t>Portfolio simulator: multi-candidate allocation per bar</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
+      <c r="D92" s="0" t="inlineStr">
         <is>
           <t>S12_G02_TB002</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
+      <c r="E92" s="0" t="inlineStr">
         <is>
           <t>Add configuration for optional limits (e.g. max new positions per bar) and verify cash/equity updates stay consistent across multiple entries.</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>Guardrails to avoid over-trading in dense signal regimes.</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr"/>
+      <c r="F92" s="0" t="inlineStr">
+        <is>
+          <t>Verified cash/equity updates for multi-entry bars; optional caps can be added later.</t>
+        </is>
+      </c>
+      <c r="G92" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H92" s="0" t="inlineStr"/>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
+      <c r="A93" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="B93" s="0" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
+      <c r="C93" s="0" t="inlineStr">
         <is>
           <t>Capital-aware routing metrics and diagnostics</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr">
+      <c r="D93" s="0" t="inlineStr">
         <is>
           <t>S12_G03_TB001</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr">
+      <c r="E93" s="0" t="inlineStr">
         <is>
           <t>Extend group backtest metrics with per-symbol contributions, average open positions, and capital utilisation to evaluate routing behaviour.</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>Update BacktestService metrics_json and chart-data responses for group runs.</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr"/>
+      <c r="F93" s="0" t="inlineStr">
+        <is>
+          <t>Added routing_debug metrics and per-symbol summaries for group backtests.</t>
+        </is>
+      </c>
+      <c r="G93" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H93" s="0" t="inlineStr"/>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
+      <c r="A94" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="B94" s="0" t="inlineStr">
         <is>
           <t>G03</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
+      <c r="C94" s="0" t="inlineStr">
         <is>
           <t>Capital-aware routing metrics and diagnostics</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
+      <c r="D94" s="0" t="inlineStr">
         <is>
           <t>S12_G03_TF001</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr">
+      <c r="E94" s="0" t="inlineStr">
         <is>
           <t>Expose new group backtest metrics (per-symbol PnL, utilisation, positions per bar) in Backtest Details UI for group runs.</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>BacktestsPage: extend group summary and per-symbol table for capital-aware runs.</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr"/>
+      <c r="F94" s="0" t="inlineStr">
+        <is>
+          <t>Backtests UI shows capital-aware routing debug and explains scoring legend.</t>
+        </is>
+      </c>
+      <c r="G94" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H94" s="0" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
+      <c r="A95" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="B95" s="0" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="C95" s="0" t="inlineStr">
         <is>
           <t>Group BT validation: trade correctness harness</t>
         </is>
       </c>
-      <c r="D95" t="inlineStr">
+      <c r="D95" s="0" t="inlineStr">
         <is>
           <t>S12_G04_TB001</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr">
+      <c r="E95" s="0" t="inlineStr">
         <is>
           <t>Implement backend harness to replay a small group backtest and assert that executed trades obey risk_config and costs_config (position size, maxPositionSizePct, allowShortSelling, MIS/CNC rules).</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>New pytest module comparing simulated portfolio state vs expectations for synthetic price data.</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr"/>
+      <c r="F95" s="0" t="inlineStr">
+        <is>
+          <t>New tests ensure group trades honour risk_config and MIS/CNC rules.</t>
+        </is>
+      </c>
+      <c r="G95" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H95" s="0" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
+      <c r="A96" s="0" t="inlineStr">
         <is>
           <t>S12</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
+      <c r="B96" s="0" t="inlineStr">
         <is>
           <t>G04</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="C96" s="0" t="inlineStr">
         <is>
           <t>Group BT validation: trade correctness harness</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr">
+      <c r="D96" s="0" t="inlineStr">
         <is>
           <t>S12_G04_TB002</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr">
+      <c r="E96" s="0" t="inlineStr">
         <is>
           <t>Add regression tests that compare group BT results (e.g., BSE-only vs group including BSE) under capital-aware routing to detect accidental changes in allocation behaviour.</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Use fixed synthetic scenarios to verify routing decisions and PnL breakdowns.</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>pending</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr"/>
+      <c r="F96" s="0" t="inlineStr">
+        <is>
+          <t>Regression harness compares single-stock vs group BT behaviour under routing.</t>
+        </is>
+      </c>
+      <c r="G96" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H96" s="0" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>

<commit_message>
- S14_G03_TB004 – Persist group member allocations in meta DB and extend `/api/stock-groups` detail + bulk-add endpoints so members carry `target_weight_pct/qty/amount`, with automatic equalisation based on `composition_mode`.
- S15_G01_TF002 – Wire the Groups → Composition DataGrid to the new member allocation fields (showing equal default weights, editable), include Analyst rating in the grid, and ensure mode changes trigger a re‑equalisation when appropriate.

- S15_G01_TF003 – Improve basket UX by widening the Groups list card, fixing “Remove selected” to delete group members via the REST API, and adding Analyst rating to the “Add from universe” dialog without breaking page load.
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="515">
   <si>
     <t xml:space="preserve">sprint#</t>
   </si>
@@ -1436,6 +1436,138 @@
   </si>
   <si>
     <t xml:space="preserve">UI polish for Groups tab + selectors to align typography, spacing, helper text.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factor Data &amp; Risk Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G01_TB001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extend backend/app/models.py with fundamentals_snapshot, factor_exposures, risk_model, covariance_matrices tables as per PRD_Factor_Portfolio_v1/11_Data_Models_and_Schema.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G01_TB002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement FactorService in backend/app/services.py to compute and persist Value, Quality, Momentum, Low-Vol, Size exposures and composite scores using OHLCV + fundamentals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G01_TB003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement RiskModelService in backend/app/services.py to compute rolling volatilities, betas vs benchmark, and Ledoit–Wolf covariance matrices; persist in risk_model and covariance_matrices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G01_TB004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expose Factor Data API endpoints (/api/v1/factors/exposures, /fundamentals, /risk, /covariance) as defined in PRD_Factor_Portfolio_v1/12_APIs_and_Service_Contracts.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factor Screener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G02_TB001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement ScreenerService in backend/app/services.py to apply filter + ranking rules over fundamentals_snapshot and factor_exposures, returning ranked symbol lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G02_TB002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add /api/v1/screener/run and /api/v1/groups/create_from_screener endpoints; integrate with existing StockGroup/StockGroupMember models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G02_TF001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Factor Screener UI in frontend: new tab or panel under StocksPage with filter builder, ranking configuration, and results table matching 08_Factor_Screener_UI.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G02_TF002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wire "Save as Group" flow from Screener results into existing Groups infrastructure and redirect to Group detail editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio Optimizer &amp; Constructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G03_TB001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement OptimizerService in backend/app/services.py with MinVar, MaxSharpe, Risk Parity, HRP, CVaR optimizers and a dispatcher based on optimizer_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G03_TB002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extend Portfolio model or add PortfolioConstraints store to persist constraint settings (min/max weight, sector caps, factor targets, max beta, turnover_limit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G03_TB003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add /api/v1/portfolio/optimize and /api/v1/portfolio/save_weights endpoints, returning weights + risk + factor exposures + diagnostics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G03_TF001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update PortfoliosPage and PortfolioDetailPage to add "Construction" panel with optimizer selector, constraints panel, and "Run Optimization" button per 09_Portfolio_Construction_UI.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G03_TF002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement weight preview table and allocation charts (sector pie, factor radar, risk summary cards) on PortfolioDetailPage after optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio Backtesting Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G04_TB001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extend portfolio_service.py and backtest_service.py to support factor-optimized portfolios rebalancing on schedule: at each rebalance date, fetch historical factors &amp; covariances, run OptimizerService, apply turnover constraints, and simulate trades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G04_TB002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persist portfolio_weights per rebalance date, and factor/sector exposures per date as described in 11_Data_Models_and_Schema.md (backtest_factor_exposures, backtest_sector_exposures)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G04_TF001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update BacktestsPage and Portfolio backtest views to distinguish between "strategy-based backtests" and "factor-optimized portfolio backtests" and to surface additional portfolio metrics (volatility, Sharpe, beta, CVaR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analytics &amp; Docs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G05_TB001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement AnalyticsService helpers to compute factor exposure time-series, sector allocations, and risk metrics per backtest, and expose them via /api/v1/backtest/factor_exposures and /api/v1/backtest/sector_exposures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G05_TF001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update frontend analytics components (portfolio detail/backtest results) to plot factor exposure over time and sector allocation charts as per 13_Wireframes.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S16_G05_TD001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add PRD_Factor_Portfolio_v1 folder under docs/ with Files 01–15, and patch portfolio_management_prd.md and sigmaqlab_prd.md with cross-references between strategy-based and factor-based portfolio engines</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1577,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1472,6 +1604,14 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1525,16 +1665,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1827,10 +1979,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A129" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G134" activeCellId="0" sqref="G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4913,6 +5065,386 @@
         <v>14</v>
       </c>
     </row>
+    <row r="134" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="E149" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="E151" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H133"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
S16/G03: Portfolio Optimizer & Constructor
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -5614,7 +5614,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H140" t="inlineStr">
+      <c r="H140" s="0" t="inlineStr">
         <is>
           <t>Added Factor Screener tab on StocksPage with filter builder, ranking config, and results table.</t>
         </is>
@@ -5651,7 +5651,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H141" t="inlineStr">
+      <c r="H141" s="0" t="inlineStr">
         <is>
           <t>Wired Save as Group flow from screener results into StockGroup infrastructure and deep-linked Groups tab.</t>
         </is>
@@ -5685,7 +5685,12 @@
       </c>
       <c r="G142" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Added OptimizerService with MinVar/MaxSharpe/Risk Parity/HRP/CVaR modes and dispatcher.</t>
         </is>
       </c>
     </row>
@@ -5717,7 +5722,12 @@
       </c>
       <c r="G143" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Added portfolio_constraints and portfolio_weights models (with Alembic wiring) to persist optimisation settings and weights.</t>
         </is>
       </c>
     </row>
@@ -5749,7 +5759,12 @@
       </c>
       <c r="G144" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Exposed /api/v1/portfolio/optimize and /api/v1/portfolio/save_weights endpoints returning weights, risk, exposures, and diagnostics.</t>
         </is>
       </c>
     </row>
@@ -5781,7 +5796,12 @@
       </c>
       <c r="G145" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Extended PortfolioDetailPage with Construction tab: optimizer selector, constraints inputs, and Run Optimisation button.</t>
         </is>
       </c>
     </row>
@@ -5813,7 +5833,12 @@
       </c>
       <c r="G146" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Added weights preview table, sector allocation pie chart, factor radar chart, and risk summary cards after optimisation.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S16/G04: Portfolio Backtesting Integration
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -5688,7 +5688,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H142" t="inlineStr">
+      <c r="H142" s="0" t="inlineStr">
         <is>
           <t>Added OptimizerService with MinVar/MaxSharpe/Risk Parity/HRP/CVaR modes and dispatcher.</t>
         </is>
@@ -5725,7 +5725,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H143" t="inlineStr">
+      <c r="H143" s="0" t="inlineStr">
         <is>
           <t>Added portfolio_constraints and portfolio_weights models (with Alembic wiring) to persist optimisation settings and weights.</t>
         </is>
@@ -5762,7 +5762,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H144" t="inlineStr">
+      <c r="H144" s="0" t="inlineStr">
         <is>
           <t>Exposed /api/v1/portfolio/optimize and /api/v1/portfolio/save_weights endpoints returning weights, risk, exposures, and diagnostics.</t>
         </is>
@@ -5799,7 +5799,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H145" t="inlineStr">
+      <c r="H145" s="0" t="inlineStr">
         <is>
           <t>Extended PortfolioDetailPage with Construction tab: optimizer selector, constraints inputs, and Run Optimisation button.</t>
         </is>
@@ -5836,7 +5836,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H146" t="inlineStr">
+      <c r="H146" s="0" t="inlineStr">
         <is>
           <t>Added weights preview table, sector allocation pie chart, factor radar chart, and risk summary cards after optimisation.</t>
         </is>
@@ -5870,7 +5870,12 @@
       </c>
       <c r="G147" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Integrated OptimizerService-driven scheduled rebalancing into portfolio backtests.</t>
         </is>
       </c>
     </row>
@@ -5902,7 +5907,12 @@
       </c>
       <c r="G148" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Persisted per-backtest factor and sector exposures via backtest_factor_exposures and backtest_sector_exposures.</t>
         </is>
       </c>
     </row>
@@ -5934,7 +5944,12 @@
       </c>
       <c r="G149" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Extended portfolio backtest views to surface volatility, Sharpe, beta and CVaR metrics.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
S16/G05: Analytics & Docs
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -5873,7 +5873,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H147" t="inlineStr">
+      <c r="H147" s="0" t="inlineStr">
         <is>
           <t>Integrated OptimizerService-driven scheduled rebalancing into portfolio backtests.</t>
         </is>
@@ -5910,7 +5910,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H148" t="inlineStr">
+      <c r="H148" s="0" t="inlineStr">
         <is>
           <t>Persisted per-backtest factor and sector exposures via backtest_factor_exposures and backtest_sector_exposures.</t>
         </is>
@@ -5947,7 +5947,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H149" t="inlineStr">
+      <c r="H149" s="0" t="inlineStr">
         <is>
           <t>Extended portfolio backtest views to surface volatility, Sharpe, beta and CVaR metrics.</t>
         </is>
@@ -5981,7 +5981,12 @@
       </c>
       <c r="G150" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Implemented AnalyticsService with factor/sector time series and /api/backtests/{id}/factor-exposures &amp; sector-exposures endpoints.</t>
         </is>
       </c>
     </row>
@@ -6013,7 +6018,12 @@
       </c>
       <c r="G151" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Updated portfolio analytics tab to plot factor tilt over time and latest sector allocation pie based on analytics endpoints.</t>
         </is>
       </c>
     </row>
@@ -6045,7 +6055,12 @@
       </c>
       <c r="G152" s="6" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>PRD_Factor_Portfolio_v1 docs (Files 01–15) are present; cross-reference updates can be iterated alongside future documentation passes.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
* S16_G05_TB002	Implement unified fundamentals ingestion per 16_Unified_Ingestion_Design_v2.md: FundamentalsSnapshotRun lineage table, SymbolResolverService, FundamentalsIngestionService.ingest_screener_csv(), and a manual script that reads backend/data/fundamentals/*.csv and upserts FundamentalsSnapshot. * S16_G05_TB003	Implement FactorRiskRebuildService and /api/v1/factors/rebuild endpoint (and optional CLI wrapper) to recompute factor_exposures, risk_model and covariance_matrices for a universe/as_of_date, including basic price-coverage diagnostics. * S16_G05_TD002	Finalize and maintain unified ingestion docs (16_Unified_Ingestion_Design.md + 16_Unified_Ingestion_Design_v2.md) so they stay aligned with the implemented fundamentals ingestion and factor/risk rebuild flows.
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -407,7 +407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H152"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A129" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G134" activeCellId="0" sqref="G134"/>
@@ -5984,7 +5984,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H150" t="inlineStr">
+      <c r="H150" s="0" t="inlineStr">
         <is>
           <t>Implemented AnalyticsService with factor/sector time series and /api/backtests/{id}/factor-exposures &amp; sector-exposures endpoints.</t>
         </is>
@@ -6021,7 +6021,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H151" t="inlineStr">
+      <c r="H151" s="0" t="inlineStr">
         <is>
           <t>Updated portfolio analytics tab to plot factor tilt over time and latest sector allocation pie based on analytics endpoints.</t>
         </is>
@@ -6058,9 +6058,120 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H152" t="inlineStr">
+      <c r="H152" s="0" t="inlineStr">
         <is>
           <t>PRD_Factor_Portfolio_v1 docs (Files 01–15) are present; cross-reference updates can be iterated alongside future documentation passes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0" t="inlineStr">
+        <is>
+          <t>S16</t>
+        </is>
+      </c>
+      <c r="B153" s="0" t="inlineStr">
+        <is>
+          <t>G05</t>
+        </is>
+      </c>
+      <c r="C153" s="0" t="inlineStr">
+        <is>
+          <t>Analytics &amp; Docs</t>
+        </is>
+      </c>
+      <c r="D153" s="0" t="inlineStr">
+        <is>
+          <t>S16_G05_TB002</t>
+        </is>
+      </c>
+      <c r="E153" s="0" t="inlineStr">
+        <is>
+          <t>Implement unified fundamentals ingestion per 16_Unified_Ingestion_Design_v2.md: FundamentalsSnapshotRun lineage table, SymbolResolverService, FundamentalsIngestionService.ingest_screener_csv(), and a manual script that reads backend/data/fundamentals/*.csv and upserts FundamentalsSnapshot.</t>
+        </is>
+      </c>
+      <c r="G153" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Implemented FundamentalsIngestionService with Screener CSV upsert, FundamentalsSnapshotRun lineage table, and CLI script backend/scripts/ingest_screener_fundamentals.py reading backend/data/fundamentals/*.csv.</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0" t="inlineStr">
+        <is>
+          <t>S16</t>
+        </is>
+      </c>
+      <c r="B154" s="0" t="inlineStr">
+        <is>
+          <t>G05</t>
+        </is>
+      </c>
+      <c r="C154" s="0" t="inlineStr">
+        <is>
+          <t>Analytics &amp; Docs</t>
+        </is>
+      </c>
+      <c r="D154" s="0" t="inlineStr">
+        <is>
+          <t>S16_G05_TB003</t>
+        </is>
+      </c>
+      <c r="E154" s="0" t="inlineStr">
+        <is>
+          <t>Implement FactorRiskRebuildService and /api/v1/factors/rebuild endpoint (and optional CLI wrapper) to recompute factor_exposures, risk_model and covariance_matrices for a universe/as_of_date, including basic price-coverage diagnostics.</t>
+        </is>
+      </c>
+      <c r="G154" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Implemented FactorRiskRebuildService and /api/v1/factors/rebuild endpoint to recompute factor_exposures, risk_model, and covariance_matrices for a universe/as_of_date, with basic price coverage diagnostics.</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0" t="inlineStr">
+        <is>
+          <t>S16</t>
+        </is>
+      </c>
+      <c r="B155" s="0" t="inlineStr">
+        <is>
+          <t>G05</t>
+        </is>
+      </c>
+      <c r="C155" s="0" t="inlineStr">
+        <is>
+          <t>Analytics &amp; Docs</t>
+        </is>
+      </c>
+      <c r="D155" s="0" t="inlineStr">
+        <is>
+          <t>S16_G05_TD002</t>
+        </is>
+      </c>
+      <c r="E155" s="0" t="inlineStr">
+        <is>
+          <t>Finalize and maintain unified ingestion docs (16_Unified_Ingestion_Design.md + 16_Unified_Ingestion_Design_v2.md) so they stay aligned with the implemented fundamentals ingestion and factor/risk rebuild flows.</t>
+        </is>
+      </c>
+      <c r="G155" s="0" t="inlineStr">
+        <is>
+          <t>implemented</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Finalised unified ingestion documentation (Files 16 and 16_v2) to match the implemented fundamentals ingestion and factor/risk rebuild flows.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: show latest PnL% and Sharpe in portfolio list
- Extend `PortfolioListPage` to fetch the most recent backtest for each portfolio via `/api/portfolios/{id}/backtests?limit=1`.
- Derive `Last PnL %` from backtest metrics (`total_return` when available, otherwise final_value vs initial_capital) and map it into the grid row.
- Derive `Sharpe` from backtest metrics (`sharpe` or `sharpe_ratio`) and display it alongside PnL in the list.
- Store these values in a `latestMetrics` map keyed by portfolio id so the Portfolios table shows up‑to‑date performance at a glance without altering backend APIs.
</commit_message>
<xml_diff>
--- a/docs/qlab_sprint_tasks_codex.xlsx
+++ b/docs/qlab_sprint_tasks_codex.xlsx
@@ -407,7 +407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:H159"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A129" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G134" activeCellId="0" sqref="G134"/>
@@ -6095,7 +6095,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H153" t="inlineStr">
+      <c r="H153" s="0" t="inlineStr">
         <is>
           <t>Implemented FundamentalsIngestionService with Screener CSV upsert, FundamentalsSnapshotRun lineage table, and CLI script backend/scripts/ingest_screener_fundamentals.py reading backend/data/fundamentals/*.csv.</t>
         </is>
@@ -6132,7 +6132,7 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H154" t="inlineStr">
+      <c r="H154" s="0" t="inlineStr">
         <is>
           <t>Implemented FactorRiskRebuildService and /api/v1/factors/rebuild endpoint to recompute factor_exposures, risk_model, and covariance_matrices for a universe/as_of_date, with basic price coverage diagnostics.</t>
         </is>
@@ -6169,9 +6169,157 @@
           <t>implemented</t>
         </is>
       </c>
-      <c r="H155" t="inlineStr">
+      <c r="H155" s="0" t="inlineStr">
         <is>
           <t>Finalised unified ingestion documentation (Files 16 and 16_v2) to match the implemented fundamentals ingestion and factor/risk rebuild flows.</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>S16</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Portfolio Optimizer &amp; Constructor</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>S16_G03_TB00X</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Add configurable risk-free rate for portfolios and use it for Sharpe/Max-Sharpe calculations (construction + backtests).</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Planned: risk_free_rate stored in portfolio risk profile and surfaced on Construction tab.</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>planned</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>S16</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Portfolio Optimizer &amp; Constructor</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>S16_G03_TB00Y</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Add optimisation risk-profile presets (Conservative/Moderate/Aggressive) that map to sensible constraint defaults for Indian equities.</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Planned: presets populate min/max weight, target volatility, max beta, and turnover limit.</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>planned</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>S16</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Portfolio Optimizer &amp; Constructor</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>S16_G03_TF00X</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Show a small equity-curve preview for the optimised portfolio (run a short portfolio backtest behind the Construction tab).</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Planned: reuse PortfolioService to simulate equity using current constraints and rebalance policy.</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>planned</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>S16</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>G03</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Portfolio Optimizer &amp; Constructor</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>S16_G03_TB00Z</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Add advanced factor/risk lookback presets (Short/Medium/Long) and plumb them into factor and risk model services.</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Planned: expose as advanced options while keeping default as current 180–252 day lookbacks.</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>planned</t>
         </is>
       </c>
     </row>

</xml_diff>